<commit_message>
tweaking spp numbers spreadsheet to match WoRMS names
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/species_numbers.xlsx
+++ b/_raw_data/xlsx/species_numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="580" windowWidth="27540" windowHeight="14720" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="2020" yWindow="160" windowWidth="29800" windowHeight="16120" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4327" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4328" uniqueCount="1667">
   <si>
     <t>Architeuthis dux</t>
   </si>
@@ -5126,9 +5126,6 @@
     <t xml:space="preserve">Oceanodroma hornbyi </t>
   </si>
   <si>
-    <t xml:space="preserve">Oceanodroma macrodactylus </t>
-  </si>
-  <si>
     <t xml:space="preserve">Oceanodroma markhami </t>
   </si>
   <si>
@@ -5178,6 +5175,33 @@
   </si>
   <si>
     <t xml:space="preserve">Puffinus tenuirostris </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna bengalensis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna bergii </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna bernsteini </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna elegans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna maximus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna sandvicensis </t>
+  </si>
+  <si>
+    <t>Oceanodroma macrodactyla</t>
+  </si>
+  <si>
+    <t>Pachyptila macgillivrayi</t>
+  </si>
+  <si>
+    <t>subspecies of salvini</t>
   </si>
 </sst>
 </file>
@@ -5375,8 +5399,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5500,7 +5532,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5513,6 +5545,10 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5525,6 +5561,10 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6225,18 +6265,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P361"/>
+  <dimension ref="A1:R361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H165" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="7" ySplit="2" topLeftCell="K280" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K191" sqref="K191"/>
+      <selection pane="bottomRight" activeCell="R286" sqref="R286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="67.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="3" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="25.6640625" bestFit="1" customWidth="1"/>
@@ -6362,7 +6403,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="28">
       <c r="A5" s="23" t="s">
         <v>1306</v>
       </c>
@@ -6397,7 +6438,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="42">
       <c r="A6" s="23" t="s">
         <v>1307</v>
       </c>
@@ -6432,7 +6473,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="28">
       <c r="A7" s="23" t="s">
         <v>1308</v>
       </c>
@@ -6467,7 +6508,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="28">
       <c r="A8" s="23" t="s">
         <v>1309</v>
       </c>
@@ -6502,7 +6543,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" ht="28">
       <c r="A9" s="23" t="s">
         <v>1310</v>
       </c>
@@ -6537,7 +6578,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="42">
       <c r="A10" s="23" t="s">
         <v>1311</v>
       </c>
@@ -6712,7 +6753,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" ht="28">
       <c r="A15" s="23" t="s">
         <v>1316</v>
       </c>
@@ -11665,7 +11706,7 @@
         <v>729</v>
       </c>
       <c r="K185" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="L185" t="s">
         <v>926</v>
@@ -11694,7 +11735,7 @@
         <v>729</v>
       </c>
       <c r="K186" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="L186" t="s">
         <v>929</v>
@@ -11723,7 +11764,7 @@
         <v>729</v>
       </c>
       <c r="K187" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="L187" t="s">
         <v>931</v>
@@ -11752,7 +11793,7 @@
         <v>729</v>
       </c>
       <c r="K188" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="L188" t="s">
         <v>933</v>
@@ -11781,7 +11822,7 @@
         <v>729</v>
       </c>
       <c r="K189" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="L189" t="s">
         <v>935</v>
@@ -11810,7 +11851,7 @@
         <v>729</v>
       </c>
       <c r="K190" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="L190" t="s">
         <v>937</v>
@@ -11839,7 +11880,7 @@
         <v>729</v>
       </c>
       <c r="K191" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="L191" t="s">
         <v>939</v>
@@ -14206,7 +14247,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="273" spans="8:16">
+    <row r="273" spans="8:18">
       <c r="H273" t="s">
         <v>586</v>
       </c>
@@ -14235,7 +14276,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="274" spans="8:16">
+    <row r="274" spans="8:18">
       <c r="H274" t="s">
         <v>586</v>
       </c>
@@ -14264,7 +14305,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="275" spans="8:16">
+    <row r="275" spans="8:18">
       <c r="H275" t="s">
         <v>586</v>
       </c>
@@ -14293,7 +14334,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="276" spans="8:16">
+    <row r="276" spans="8:18">
       <c r="H276" t="s">
         <v>586</v>
       </c>
@@ -14322,7 +14363,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="277" spans="8:16">
+    <row r="277" spans="8:18">
       <c r="H277" t="s">
         <v>586</v>
       </c>
@@ -14351,7 +14392,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="278" spans="8:16">
+    <row r="278" spans="8:18">
       <c r="H278" t="s">
         <v>586</v>
       </c>
@@ -14380,7 +14421,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="279" spans="8:16">
+    <row r="279" spans="8:18">
       <c r="H279" t="s">
         <v>586</v>
       </c>
@@ -14409,7 +14450,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="280" spans="8:16">
+    <row r="280" spans="8:18">
       <c r="H280" t="s">
         <v>533</v>
       </c>
@@ -14438,7 +14479,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="281" spans="8:16">
+    <row r="281" spans="8:18">
       <c r="H281" t="s">
         <v>533</v>
       </c>
@@ -14467,7 +14508,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="282" spans="8:16">
+    <row r="282" spans="8:18">
       <c r="H282" t="s">
         <v>533</v>
       </c>
@@ -14496,7 +14537,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="283" spans="8:16">
+    <row r="283" spans="8:18">
       <c r="H283" t="s">
         <v>533</v>
       </c>
@@ -14525,7 +14566,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="284" spans="8:16">
+    <row r="284" spans="8:18">
       <c r="H284" t="s">
         <v>533</v>
       </c>
@@ -14554,7 +14595,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="285" spans="8:16">
+    <row r="285" spans="8:18">
       <c r="H285" t="s">
         <v>533</v>
       </c>
@@ -14583,7 +14624,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="286" spans="8:16">
+    <row r="286" spans="8:18">
       <c r="H286" t="s">
         <v>533</v>
       </c>
@@ -14594,7 +14635,7 @@
         <v>729</v>
       </c>
       <c r="K286" t="s">
-        <v>1144</v>
+        <v>1152</v>
       </c>
       <c r="L286" t="s">
         <v>1144</v>
@@ -14612,7 +14653,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="287" spans="8:16">
+    <row r="287" spans="8:18">
       <c r="H287" t="s">
         <v>533</v>
       </c>
@@ -14641,7 +14682,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="288" spans="8:16">
+    <row r="288" spans="8:18">
       <c r="H288" t="s">
         <v>533</v>
       </c>
@@ -14652,7 +14693,7 @@
         <v>729</v>
       </c>
       <c r="K288" t="s">
-        <v>1148</v>
+        <v>1665</v>
       </c>
       <c r="L288" t="s">
         <v>1148</v>
@@ -14668,6 +14709,9 @@
       </c>
       <c r="P288" t="s">
         <v>1133</v>
+      </c>
+      <c r="R288" t="s">
+        <v>1666</v>
       </c>
     </row>
     <row r="289" spans="8:16">
@@ -14791,7 +14835,7 @@
         <v>533</v>
       </c>
       <c r="I293" s="45" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J293" t="s">
         <v>729</v>
@@ -14820,7 +14864,7 @@
         <v>533</v>
       </c>
       <c r="I294" s="45" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J294" t="s">
         <v>729</v>
@@ -14849,7 +14893,7 @@
         <v>533</v>
       </c>
       <c r="I295" s="45" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J295" t="s">
         <v>729</v>
@@ -14878,7 +14922,7 @@
         <v>533</v>
       </c>
       <c r="I296" s="45" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J296" t="s">
         <v>729</v>
@@ -14936,7 +14980,7 @@
         <v>533</v>
       </c>
       <c r="I298" t="s">
-        <v>1168</v>
+        <v>1178</v>
       </c>
       <c r="J298" t="s">
         <v>1168</v>
@@ -14965,7 +15009,7 @@
         <v>533</v>
       </c>
       <c r="I299" t="s">
-        <v>1168</v>
+        <v>1178</v>
       </c>
       <c r="J299" t="s">
         <v>1168</v>
@@ -14994,7 +15038,7 @@
         <v>533</v>
       </c>
       <c r="I300" t="s">
-        <v>1168</v>
+        <v>1178</v>
       </c>
       <c r="J300" t="s">
         <v>1168</v>
@@ -15023,7 +15067,7 @@
         <v>533</v>
       </c>
       <c r="I301" t="s">
-        <v>1168</v>
+        <v>1178</v>
       </c>
       <c r="J301" t="s">
         <v>1168</v>
@@ -15174,7 +15218,7 @@
         <v>1178</v>
       </c>
       <c r="K306" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="L306" t="s">
         <v>1188</v>
@@ -15203,7 +15247,7 @@
         <v>1178</v>
       </c>
       <c r="K307" t="s">
-        <v>1641</v>
+        <v>1664</v>
       </c>
       <c r="L307" t="s">
         <v>1190</v>
@@ -15232,7 +15276,7 @@
         <v>1178</v>
       </c>
       <c r="K308" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="L308" t="s">
         <v>1192</v>
@@ -15261,7 +15305,7 @@
         <v>1178</v>
       </c>
       <c r="K309" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="L309" t="s">
         <v>1194</v>
@@ -15290,7 +15334,7 @@
         <v>1178</v>
       </c>
       <c r="K310" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="L310" t="s">
         <v>1196</v>
@@ -15319,7 +15363,7 @@
         <v>1178</v>
       </c>
       <c r="K311" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="L311" t="s">
         <v>1198</v>
@@ -15348,7 +15392,7 @@
         <v>1178</v>
       </c>
       <c r="K312" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="L312" t="s">
         <v>1200</v>
@@ -15377,7 +15421,7 @@
         <v>1178</v>
       </c>
       <c r="K313" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="L313" t="s">
         <v>1202</v>
@@ -15435,7 +15479,7 @@
         <v>1178</v>
       </c>
       <c r="K315" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="L315" t="s">
         <v>1206</v>
@@ -15464,7 +15508,7 @@
         <v>1178</v>
       </c>
       <c r="K316" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="L316" t="s">
         <v>1208</v>
@@ -16624,7 +16668,7 @@
         <v>830</v>
       </c>
       <c r="K356" t="s">
-        <v>1289</v>
+        <v>1658</v>
       </c>
       <c r="L356" t="s">
         <v>1289</v>
@@ -16653,7 +16697,7 @@
         <v>830</v>
       </c>
       <c r="K357" t="s">
-        <v>1291</v>
+        <v>1659</v>
       </c>
       <c r="L357" t="s">
         <v>1291</v>
@@ -16682,7 +16726,7 @@
         <v>830</v>
       </c>
       <c r="K358" t="s">
-        <v>1293</v>
+        <v>1660</v>
       </c>
       <c r="L358" t="s">
         <v>1293</v>
@@ -16711,7 +16755,7 @@
         <v>830</v>
       </c>
       <c r="K359" t="s">
-        <v>1295</v>
+        <v>1661</v>
       </c>
       <c r="L359" t="s">
         <v>1295</v>
@@ -16740,7 +16784,7 @@
         <v>830</v>
       </c>
       <c r="K360" t="s">
-        <v>1297</v>
+        <v>1662</v>
       </c>
       <c r="L360" t="s">
         <v>1297</v>
@@ -16769,7 +16813,7 @@
         <v>830</v>
       </c>
       <c r="K361" t="s">
-        <v>1299</v>
+        <v>1663</v>
       </c>
       <c r="L361" t="s">
         <v>1299</v>

</xml_diff>

<commit_message>
added code to create a blank csv for experts to fill out representativeness
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/species_numbers.xlsx
+++ b/_raw_data/xlsx/species_numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="2100" windowWidth="27480" windowHeight="16120" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="4560" yWindow="3060" windowWidth="27480" windowHeight="16140" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4348" uniqueCount="1687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4348" uniqueCount="1689">
   <si>
     <t>Architeuthis dux</t>
   </si>
@@ -5216,9 +5216,6 @@
     <t>WoRMS considers freshwater, not marine</t>
   </si>
   <si>
-    <t>not matching but correct... try again?</t>
-  </si>
-  <si>
     <t>Stercorarius antarcticus</t>
   </si>
   <si>
@@ -5262,6 +5259,15 @@
   </si>
   <si>
     <t>Sterna maxima</t>
+  </si>
+  <si>
+    <t>genus Anous not included in spp traits so no direct match</t>
+  </si>
+  <si>
+    <t>genus Gygis not included in spp traits so no direct match</t>
+  </si>
+  <si>
+    <t>Crowned cormorant is marine, but WoRMS considers it synonymous with Reed cormorant which WoRMS considers freshwater, not marine</t>
   </si>
 </sst>
 </file>
@@ -5459,7 +5465,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5496,6 +5502,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5608,7 +5620,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="35"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="54">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5638,6 +5650,12 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6380,10 +6398,10 @@
   <dimension ref="A1:R361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="I304" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K319" sqref="K319"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6801,7 +6819,7 @@
         <v>1222</v>
       </c>
       <c r="R11" t="s">
-        <v>1671</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -6843,7 +6861,7 @@
         <v>1222</v>
       </c>
       <c r="R12" t="s">
-        <v>1671</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -6885,7 +6903,7 @@
         <v>1222</v>
       </c>
       <c r="R13" t="s">
-        <v>1671</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -7418,7 +7436,7 @@
         <v>1115</v>
       </c>
       <c r="K29" s="46" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="L29" t="s">
         <v>1116</v>
@@ -7451,7 +7469,7 @@
         <v>1115</v>
       </c>
       <c r="K30" s="46" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="L30" t="s">
         <v>1119</v>
@@ -7484,7 +7502,7 @@
         <v>1115</v>
       </c>
       <c r="K31" s="46" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="L31" t="s">
         <v>1121</v>
@@ -7517,7 +7535,7 @@
         <v>1115</v>
       </c>
       <c r="K32" s="46" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="L32" t="s">
         <v>1123</v>
@@ -7847,7 +7865,7 @@
         <v>534</v>
       </c>
       <c r="K42" s="46" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="L42" t="s">
         <v>535</v>
@@ -8939,7 +8957,7 @@
         <v>830</v>
       </c>
       <c r="K75" s="46" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="L75" t="s">
         <v>1231</v>
@@ -9030,7 +9048,7 @@
         <v>1222</v>
       </c>
       <c r="R77" t="s">
-        <v>1671</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="78" spans="8:18">
@@ -9044,7 +9062,7 @@
         <v>830</v>
       </c>
       <c r="K78" s="46" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="L78" t="s">
         <v>1237</v>
@@ -9066,7 +9084,7 @@
         <v>1222</v>
       </c>
       <c r="R78" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="79" spans="8:18">
@@ -10862,7 +10880,7 @@
         <v>1049</v>
       </c>
       <c r="K133" s="46" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="L133" t="s">
         <v>1071</v>
@@ -11184,7 +11202,7 @@
         <v>1171</v>
       </c>
       <c r="R142" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="143" spans="8:18">
@@ -12476,6 +12494,9 @@
       <c r="Q181" t="s">
         <v>642</v>
       </c>
+      <c r="R181" t="s">
+        <v>1688</v>
+      </c>
     </row>
     <row r="182" spans="8:18">
       <c r="H182" t="s">
@@ -15420,7 +15441,7 @@
         <v>928</v>
       </c>
       <c r="R270" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="271" spans="8:18">
@@ -15456,7 +15477,7 @@
         <v>928</v>
       </c>
       <c r="R271" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="272" spans="8:18">
@@ -15590,9 +15611,6 @@
       <c r="Q275" t="s">
         <v>928</v>
       </c>
-      <c r="R275" t="s">
-        <v>1671</v>
-      </c>
     </row>
     <row r="276" spans="8:18">
       <c r="H276" t="s">
@@ -15792,7 +15810,7 @@
         <v>928</v>
       </c>
       <c r="R281" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="282" spans="8:18">
@@ -15905,7 +15923,7 @@
         <v>729</v>
       </c>
       <c r="K285" s="46" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="L285" t="s">
         <v>991</v>
@@ -16092,7 +16110,7 @@
         <v>928</v>
       </c>
       <c r="R290" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="291" spans="8:18">
@@ -17000,7 +17018,7 @@
         <v>830</v>
       </c>
       <c r="K318" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="L318" t="s">
         <v>1297</v>
@@ -21420,7 +21438,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
a couple more bird name fixes
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/species_numbers.xlsx
+++ b/_raw_data/xlsx/species_numbers.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4348" uniqueCount="1689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="1692">
   <si>
     <t>Architeuthis dux</t>
   </si>
@@ -5268,6 +5268,15 @@
   </si>
   <si>
     <t>Crowned cormorant is marine, but WoRMS considers it synonymous with Reed cormorant which WoRMS considers freshwater, not marine</t>
+  </si>
+  <si>
+    <t>Chroicocephalus genei</t>
+  </si>
+  <si>
+    <t>phaetusa simplex</t>
+  </si>
+  <si>
+    <t>Large-billed tern</t>
   </si>
 </sst>
 </file>
@@ -5614,11 +5623,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="35"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="35"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5676,7 +5685,17 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5999,7 +6018,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6395,13 +6414,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R361"/>
+  <dimension ref="A1:R362"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="H348" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="N362" sqref="N362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6491,7 +6510,7 @@
         <v>588</v>
       </c>
       <c r="M3" t="b">
-        <f>OR(K3&lt;&gt;L3,I3&lt;&gt;J3)</f>
+        <f t="shared" ref="M3:M66" si="0">OR(K3&lt;&gt;L3,I3&lt;&gt;J3)</f>
         <v>0</v>
       </c>
       <c r="N3" t="s">
@@ -6530,7 +6549,7 @@
         <v>591</v>
       </c>
       <c r="M4" t="b">
-        <f>OR(K4&lt;&gt;L4,I4&lt;&gt;J4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" t="s">
@@ -6569,7 +6588,7 @@
         <v>593</v>
       </c>
       <c r="M5" t="b">
-        <f>OR(K5&lt;&gt;L5,I5&lt;&gt;J5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" t="s">
@@ -6608,7 +6627,7 @@
         <v>595</v>
       </c>
       <c r="M6" t="b">
-        <f>OR(K6&lt;&gt;L6,I6&lt;&gt;J6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N6" t="s">
@@ -6647,7 +6666,7 @@
         <v>597</v>
       </c>
       <c r="M7" t="b">
-        <f>OR(K7&lt;&gt;L7,I7&lt;&gt;J7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7" t="s">
@@ -6686,7 +6705,7 @@
         <v>599</v>
       </c>
       <c r="M8" t="b">
-        <f>OR(K8&lt;&gt;L8,I8&lt;&gt;J8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8" t="s">
@@ -6725,7 +6744,7 @@
         <v>1251</v>
       </c>
       <c r="M9" t="b">
-        <f>OR(K9&lt;&gt;L9,I9&lt;&gt;J9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" t="s">
@@ -6764,7 +6783,7 @@
         <v>1253</v>
       </c>
       <c r="M10" t="b">
-        <f>OR(K10&lt;&gt;L10,I10&lt;&gt;J10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" t="s">
@@ -6803,7 +6822,7 @@
         <v>1220</v>
       </c>
       <c r="M11" t="b">
-        <f>OR(K11&lt;&gt;L11,I11&lt;&gt;J11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" t="s">
@@ -6845,7 +6864,7 @@
         <v>1223</v>
       </c>
       <c r="M12" t="b">
-        <f>OR(K12&lt;&gt;L12,I12&lt;&gt;J12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N12" t="s">
@@ -6887,7 +6906,7 @@
         <v>1225</v>
       </c>
       <c r="M13" t="b">
-        <f>OR(K13&lt;&gt;L13,I13&lt;&gt;J13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" t="s">
@@ -6929,7 +6948,7 @@
         <v>1131</v>
       </c>
       <c r="M14" t="b">
-        <f>OR(K14&lt;&gt;L14,I14&lt;&gt;J14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" t="s">
@@ -6968,7 +6987,7 @@
         <v>1005</v>
       </c>
       <c r="M15" t="b">
-        <f>OR(K15&lt;&gt;L15,I15&lt;&gt;J15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" t="s">
@@ -7007,7 +7026,7 @@
         <v>1008</v>
       </c>
       <c r="M16" t="b">
-        <f>OR(K16&lt;&gt;L16,I16&lt;&gt;J16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" t="s">
@@ -7040,7 +7059,7 @@
         <v>1050</v>
       </c>
       <c r="M17" t="b">
-        <f>OR(K17&lt;&gt;L17,I17&lt;&gt;J17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N17" t="s">
@@ -7073,7 +7092,7 @@
         <v>601</v>
       </c>
       <c r="M18" t="b">
-        <f>OR(K18&lt;&gt;L18,I18&lt;&gt;J18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N18" t="s">
@@ -7106,7 +7125,7 @@
         <v>603</v>
       </c>
       <c r="M19" t="b">
-        <f>OR(K19&lt;&gt;L19,I19&lt;&gt;J19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19" t="s">
@@ -7139,7 +7158,7 @@
         <v>605</v>
       </c>
       <c r="M20" t="b">
-        <f>OR(K20&lt;&gt;L20,I20&lt;&gt;J20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N20" t="s">
@@ -7172,7 +7191,7 @@
         <v>1053</v>
       </c>
       <c r="M21" t="b">
-        <f>OR(K21&lt;&gt;L21,I21&lt;&gt;J21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N21" t="s">
@@ -7208,7 +7227,7 @@
         <v>1055</v>
       </c>
       <c r="M22" t="b">
-        <f>OR(K22&lt;&gt;L22,I22&lt;&gt;J22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N22" t="s">
@@ -7244,7 +7263,7 @@
         <v>1134</v>
       </c>
       <c r="M23" t="b">
-        <f>OR(K23&lt;&gt;L23,I23&lt;&gt;J23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N23" t="s">
@@ -7277,7 +7296,7 @@
         <v>1136</v>
       </c>
       <c r="M24" t="b">
-        <f>OR(K24&lt;&gt;L24,I24&lt;&gt;J24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N24" t="s">
@@ -7310,7 +7329,7 @@
         <v>941</v>
       </c>
       <c r="M25" t="b">
-        <f>OR(K25&lt;&gt;L25,I25&lt;&gt;J25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N25" t="s">
@@ -7343,7 +7362,7 @@
         <v>943</v>
       </c>
       <c r="M26" t="b">
-        <f>OR(K26&lt;&gt;L26,I26&lt;&gt;J26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N26" t="s">
@@ -7376,7 +7395,7 @@
         <v>945</v>
       </c>
       <c r="M27" t="b">
-        <f>OR(K27&lt;&gt;L27,I27&lt;&gt;J27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N27" t="s">
@@ -7409,7 +7428,7 @@
         <v>947</v>
       </c>
       <c r="M28" t="b">
-        <f>OR(K28&lt;&gt;L28,I28&lt;&gt;J28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N28" t="s">
@@ -7435,14 +7454,14 @@
       <c r="J29" t="s">
         <v>1115</v>
       </c>
-      <c r="K29" s="46" t="s">
+      <c r="K29" s="45" t="s">
         <v>1671</v>
       </c>
       <c r="L29" t="s">
         <v>1116</v>
       </c>
       <c r="M29" t="b">
-        <f>OR(K29&lt;&gt;L29,I29&lt;&gt;J29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N29" t="s">
@@ -7468,14 +7487,14 @@
       <c r="J30" t="s">
         <v>1115</v>
       </c>
-      <c r="K30" s="46" t="s">
+      <c r="K30" s="45" t="s">
         <v>1672</v>
       </c>
       <c r="L30" t="s">
         <v>1119</v>
       </c>
       <c r="M30" t="b">
-        <f>OR(K30&lt;&gt;L30,I30&lt;&gt;J30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N30" t="s">
@@ -7501,14 +7520,14 @@
       <c r="J31" t="s">
         <v>1115</v>
       </c>
-      <c r="K31" s="46" t="s">
+      <c r="K31" s="45" t="s">
         <v>1673</v>
       </c>
       <c r="L31" t="s">
         <v>1121</v>
       </c>
       <c r="M31" t="b">
-        <f>OR(K31&lt;&gt;L31,I31&lt;&gt;J31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N31" t="s">
@@ -7534,14 +7553,14 @@
       <c r="J32" t="s">
         <v>1115</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="K32" s="45" t="s">
         <v>1674</v>
       </c>
       <c r="L32" t="s">
         <v>1123</v>
       </c>
       <c r="M32" t="b">
-        <f>OR(K32&lt;&gt;L32,I32&lt;&gt;J32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N32" t="s">
@@ -7574,7 +7593,7 @@
         <v>607</v>
       </c>
       <c r="M33" t="b">
-        <f>OR(K33&lt;&gt;L33,I33&lt;&gt;J33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N33" t="s">
@@ -7607,7 +7626,7 @@
         <v>609</v>
       </c>
       <c r="M34" t="b">
-        <f>OR(K34&lt;&gt;L34,I34&lt;&gt;J34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N34" t="s">
@@ -7640,7 +7659,7 @@
         <v>611</v>
       </c>
       <c r="M35" t="b">
-        <f>OR(K35&lt;&gt;L35,I35&lt;&gt;J35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N35" t="s">
@@ -7673,7 +7692,7 @@
         <v>613</v>
       </c>
       <c r="M36" t="b">
-        <f>OR(K36&lt;&gt;L36,I36&lt;&gt;J36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N36" t="s">
@@ -7706,7 +7725,7 @@
         <v>1227</v>
       </c>
       <c r="M37" t="b">
-        <f>OR(K37&lt;&gt;L37,I37&lt;&gt;J37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N37" t="s">
@@ -7739,7 +7758,7 @@
         <v>1229</v>
       </c>
       <c r="M38" t="b">
-        <f>OR(K38&lt;&gt;L38,I38&lt;&gt;J38)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N38" t="s">
@@ -7772,7 +7791,7 @@
         <v>1057</v>
       </c>
       <c r="M39" t="b">
-        <f>OR(K39&lt;&gt;L39,I39&lt;&gt;J39)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N39" t="s">
@@ -7805,7 +7824,7 @@
         <v>831</v>
       </c>
       <c r="M40" t="b">
-        <f>OR(K40&lt;&gt;L40,I40&lt;&gt;J40)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N40" t="s">
@@ -7838,7 +7857,7 @@
         <v>1138</v>
       </c>
       <c r="M41" t="b">
-        <f>OR(K41&lt;&gt;L41,I41&lt;&gt;J41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N41" t="s">
@@ -7864,14 +7883,14 @@
       <c r="J42" t="s">
         <v>534</v>
       </c>
-      <c r="K42" s="46" t="s">
+      <c r="K42" s="45" t="s">
         <v>1675</v>
       </c>
       <c r="L42" t="s">
         <v>535</v>
       </c>
       <c r="M42" t="b">
-        <f>OR(K42&lt;&gt;L42,I42&lt;&gt;J42)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N42" t="s">
@@ -7907,7 +7926,7 @@
         <v>540</v>
       </c>
       <c r="M43" t="b">
-        <f>OR(K43&lt;&gt;L43,I43&lt;&gt;J43)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N43" t="s">
@@ -7940,7 +7959,7 @@
         <v>542</v>
       </c>
       <c r="M44" t="b">
-        <f>OR(K44&lt;&gt;L44,I44&lt;&gt;J44)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N44" t="s">
@@ -7973,7 +7992,7 @@
         <v>545</v>
       </c>
       <c r="M45" t="b">
-        <f>OR(K45&lt;&gt;L45,I45&lt;&gt;J45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N45" t="s">
@@ -8006,7 +8025,7 @@
         <v>548</v>
       </c>
       <c r="M46" t="b">
-        <f>OR(K46&lt;&gt;L46,I46&lt;&gt;J46)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N46" t="s">
@@ -8039,7 +8058,7 @@
         <v>550</v>
       </c>
       <c r="M47" t="b">
-        <f>OR(K47&lt;&gt;L47,I47&lt;&gt;J47)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N47" t="s">
@@ -8072,7 +8091,7 @@
         <v>1010</v>
       </c>
       <c r="M48" t="b">
-        <f>OR(K48&lt;&gt;L48,I48&lt;&gt;J48)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N48" t="s">
@@ -8105,7 +8124,7 @@
         <v>1012</v>
       </c>
       <c r="M49" t="b">
-        <f>OR(K49&lt;&gt;L49,I49&lt;&gt;J49)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N49" t="s">
@@ -8138,7 +8157,7 @@
         <v>1014</v>
       </c>
       <c r="M50" t="b">
-        <f>OR(K50&lt;&gt;L50,I50&lt;&gt;J50)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N50" t="s">
@@ -8171,7 +8190,7 @@
         <v>1016</v>
       </c>
       <c r="M51" t="b">
-        <f>OR(K51&lt;&gt;L51,I51&lt;&gt;J51)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N51" t="s">
@@ -8204,7 +8223,7 @@
         <v>1018</v>
       </c>
       <c r="M52" t="b">
-        <f>OR(K52&lt;&gt;L52,I52&lt;&gt;J52)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N52" t="s">
@@ -8237,7 +8256,7 @@
         <v>1020</v>
       </c>
       <c r="M53" t="b">
-        <f>OR(K53&lt;&gt;L53,I53&lt;&gt;J53)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N53" t="s">
@@ -8270,7 +8289,7 @@
         <v>1022</v>
       </c>
       <c r="M54" t="b">
-        <f>OR(K54&lt;&gt;L54,I54&lt;&gt;J54)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N54" t="s">
@@ -8303,7 +8322,7 @@
         <v>1024</v>
       </c>
       <c r="M55" t="b">
-        <f>OR(K55&lt;&gt;L55,I55&lt;&gt;J55)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N55" t="s">
@@ -8336,7 +8355,7 @@
         <v>615</v>
       </c>
       <c r="M56" t="b">
-        <f>OR(K56&lt;&gt;L56,I56&lt;&gt;J56)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N56" t="s">
@@ -8369,7 +8388,7 @@
         <v>617</v>
       </c>
       <c r="M57" t="b">
-        <f>OR(K57&lt;&gt;L57,I57&lt;&gt;J57)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N57" t="s">
@@ -8402,7 +8421,7 @@
         <v>619</v>
       </c>
       <c r="M58" t="b">
-        <f>OR(K58&lt;&gt;L58,I58&lt;&gt;J58)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N58" t="s">
@@ -8435,7 +8454,7 @@
         <v>719</v>
       </c>
       <c r="M59" t="b">
-        <f>OR(K59&lt;&gt;L59,I59&lt;&gt;J59)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N59" t="s">
@@ -8468,7 +8487,7 @@
         <v>721</v>
       </c>
       <c r="M60" t="b">
-        <f>OR(K60&lt;&gt;L60,I60&lt;&gt;J60)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N60" t="s">
@@ -8501,7 +8520,7 @@
         <v>723</v>
       </c>
       <c r="M61" t="b">
-        <f>OR(K61&lt;&gt;L61,I61&lt;&gt;J61)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N61" t="s">
@@ -8534,7 +8553,7 @@
         <v>725</v>
       </c>
       <c r="M62" t="b">
-        <f>OR(K62&lt;&gt;L62,I62&lt;&gt;J62)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N62" t="s">
@@ -8567,7 +8586,7 @@
         <v>727</v>
       </c>
       <c r="M63" t="b">
-        <f>OR(K63&lt;&gt;L63,I63&lt;&gt;J63)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N63" t="s">
@@ -8600,7 +8619,7 @@
         <v>1169</v>
       </c>
       <c r="M64" t="b">
-        <f>OR(K64&lt;&gt;L64,I64&lt;&gt;J64)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N64" t="s">
@@ -8633,7 +8652,7 @@
         <v>1172</v>
       </c>
       <c r="M65" t="b">
-        <f>OR(K65&lt;&gt;L65,I65&lt;&gt;J65)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N65" t="s">
@@ -8666,7 +8685,7 @@
         <v>1174</v>
       </c>
       <c r="M66" t="b">
-        <f>OR(K66&lt;&gt;L66,I66&lt;&gt;J66)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N66" t="s">
@@ -8699,7 +8718,7 @@
         <v>949</v>
       </c>
       <c r="M67" t="b">
-        <f>OR(K67&lt;&gt;L67,I67&lt;&gt;J67)</f>
+        <f t="shared" ref="M67:M130" si="1">OR(K67&lt;&gt;L67,I67&lt;&gt;J67)</f>
         <v>0</v>
       </c>
       <c r="N67" t="s">
@@ -8732,7 +8751,7 @@
         <v>951</v>
       </c>
       <c r="M68" t="b">
-        <f>OR(K68&lt;&gt;L68,I68&lt;&gt;J68)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N68" t="s">
@@ -8765,7 +8784,7 @@
         <v>1176</v>
       </c>
       <c r="M69" t="b">
-        <f>OR(K69&lt;&gt;L69,I69&lt;&gt;J69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N69" t="s">
@@ -8798,7 +8817,7 @@
         <v>1095</v>
       </c>
       <c r="M70" t="b">
-        <f>OR(K70&lt;&gt;L70,I70&lt;&gt;J70)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N70" t="s">
@@ -8831,7 +8850,7 @@
         <v>1097</v>
       </c>
       <c r="M71" t="b">
-        <f>OR(K71&lt;&gt;L71,I71&lt;&gt;J71)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N71" t="s">
@@ -8864,7 +8883,7 @@
         <v>1099</v>
       </c>
       <c r="M72" t="b">
-        <f>OR(K72&lt;&gt;L72,I72&lt;&gt;J72)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N72" t="s">
@@ -8897,7 +8916,7 @@
         <v>1101</v>
       </c>
       <c r="M73" t="b">
-        <f>OR(K73&lt;&gt;L73,I73&lt;&gt;J73)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N73" t="s">
@@ -8930,7 +8949,7 @@
         <v>1103</v>
       </c>
       <c r="M74" t="b">
-        <f>OR(K74&lt;&gt;L74,I74&lt;&gt;J74)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N74" t="s">
@@ -8956,14 +8975,14 @@
       <c r="J75" t="s">
         <v>830</v>
       </c>
-      <c r="K75" s="46" t="s">
+      <c r="K75" s="45" t="s">
         <v>1676</v>
       </c>
       <c r="L75" t="s">
         <v>1231</v>
       </c>
       <c r="M75" t="b">
-        <f>OR(K75&lt;&gt;L75,I75&lt;&gt;J75)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N75" t="s">
@@ -8999,7 +9018,7 @@
         <v>1233</v>
       </c>
       <c r="M76" t="b">
-        <f>OR(K76&lt;&gt;L76,I76&lt;&gt;J76)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N76" t="s">
@@ -9032,7 +9051,7 @@
         <v>1235</v>
       </c>
       <c r="M77" t="b">
-        <f>OR(K77&lt;&gt;L77,I77&lt;&gt;J77)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N77" t="s">
@@ -9061,14 +9080,14 @@
       <c r="J78" t="s">
         <v>830</v>
       </c>
-      <c r="K78" s="46" t="s">
+      <c r="K78" s="45" t="s">
         <v>1678</v>
       </c>
       <c r="L78" t="s">
         <v>1237</v>
       </c>
       <c r="M78" t="b">
-        <f>OR(K78&lt;&gt;L78,I78&lt;&gt;J78)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N78" t="s">
@@ -9104,7 +9123,7 @@
         <v>1140</v>
       </c>
       <c r="M79" t="b">
-        <f>OR(K79&lt;&gt;L79,I79&lt;&gt;J79)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N79" t="s">
@@ -9137,7 +9156,7 @@
         <v>1059</v>
       </c>
       <c r="M80" t="b">
-        <f>OR(K80&lt;&gt;L80,I80&lt;&gt;J80)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N80" t="s">
@@ -9170,7 +9189,7 @@
         <v>1181</v>
       </c>
       <c r="M81" t="b">
-        <f>OR(K81&lt;&gt;L81,I81&lt;&gt;J81)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N81" t="s">
@@ -9203,7 +9222,7 @@
         <v>1204</v>
       </c>
       <c r="M82" t="b">
-        <f>OR(K82&lt;&gt;L82,I82&lt;&gt;J82)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N82" t="s">
@@ -9236,7 +9255,7 @@
         <v>834</v>
       </c>
       <c r="M83" t="b">
-        <f>OR(K83&lt;&gt;L83,I83&lt;&gt;J83)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N83" t="s">
@@ -9269,7 +9288,7 @@
         <v>1239</v>
       </c>
       <c r="M84" t="b">
-        <f>OR(K84&lt;&gt;L84,I84&lt;&gt;J84)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N84" t="s">
@@ -9302,7 +9321,7 @@
         <v>1241</v>
       </c>
       <c r="M85" t="b">
-        <f>OR(K85&lt;&gt;L85,I85&lt;&gt;J85)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N85" t="s">
@@ -9335,7 +9354,7 @@
         <v>836</v>
       </c>
       <c r="M86" t="b">
-        <f>OR(K86&lt;&gt;L86,I86&lt;&gt;J86)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N86" t="s">
@@ -9368,7 +9387,7 @@
         <v>838</v>
       </c>
       <c r="M87" t="b">
-        <f>OR(K87&lt;&gt;L87,I87&lt;&gt;J87)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N87" t="s">
@@ -9401,7 +9420,7 @@
         <v>840</v>
       </c>
       <c r="M88" t="b">
-        <f>OR(K88&lt;&gt;L88,I88&lt;&gt;J88)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N88" t="s">
@@ -9434,7 +9453,7 @@
         <v>842</v>
       </c>
       <c r="M89" t="b">
-        <f>OR(K89&lt;&gt;L89,I89&lt;&gt;J89)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N89" t="s">
@@ -9467,7 +9486,7 @@
         <v>844</v>
       </c>
       <c r="M90" t="b">
-        <f>OR(K90&lt;&gt;L90,I90&lt;&gt;J90)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N90" t="s">
@@ -9500,7 +9519,7 @@
         <v>846</v>
       </c>
       <c r="M91" t="b">
-        <f>OR(K91&lt;&gt;L91,I91&lt;&gt;J91)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N91" t="s">
@@ -9533,7 +9552,7 @@
         <v>848</v>
       </c>
       <c r="M92" t="b">
-        <f>OR(K92&lt;&gt;L92,I92&lt;&gt;J92)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N92" t="s">
@@ -9566,7 +9585,7 @@
         <v>850</v>
       </c>
       <c r="M93" t="b">
-        <f>OR(K93&lt;&gt;L93,I93&lt;&gt;J93)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N93" t="s">
@@ -9599,7 +9618,7 @@
         <v>852</v>
       </c>
       <c r="M94" t="b">
-        <f>OR(K94&lt;&gt;L94,I94&lt;&gt;J94)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N94" t="s">
@@ -9632,7 +9651,7 @@
         <v>854</v>
       </c>
       <c r="M95" t="b">
-        <f>OR(K95&lt;&gt;L95,I95&lt;&gt;J95)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N95" t="s">
@@ -9665,7 +9684,7 @@
         <v>856</v>
       </c>
       <c r="M96" t="b">
-        <f>OR(K96&lt;&gt;L96,I96&lt;&gt;J96)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N96" t="s">
@@ -9698,7 +9717,7 @@
         <v>858</v>
       </c>
       <c r="M97" t="b">
-        <f>OR(K97&lt;&gt;L97,I97&lt;&gt;J97)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N97" t="s">
@@ -9731,7 +9750,7 @@
         <v>860</v>
       </c>
       <c r="M98" t="b">
-        <f>OR(K98&lt;&gt;L98,I98&lt;&gt;J98)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N98" t="s">
@@ -9764,7 +9783,7 @@
         <v>862</v>
       </c>
       <c r="M99" t="b">
-        <f>OR(K99&lt;&gt;L99,I99&lt;&gt;J99)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N99" t="s">
@@ -9797,7 +9816,7 @@
         <v>864</v>
       </c>
       <c r="M100" t="b">
-        <f>OR(K100&lt;&gt;L100,I100&lt;&gt;J100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N100" t="s">
@@ -9824,14 +9843,14 @@
         <v>830</v>
       </c>
       <c r="K101" t="s">
-        <v>866</v>
+        <v>1689</v>
       </c>
       <c r="L101" t="s">
         <v>866</v>
       </c>
       <c r="M101" t="b">
-        <f>OR(K101&lt;&gt;L101,I101&lt;&gt;J101)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="N101" t="s">
         <v>867</v>
@@ -9863,7 +9882,7 @@
         <v>868</v>
       </c>
       <c r="M102" t="b">
-        <f>OR(K102&lt;&gt;L102,I102&lt;&gt;J102)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N102" t="s">
@@ -9896,7 +9915,7 @@
         <v>870</v>
       </c>
       <c r="M103" t="b">
-        <f>OR(K103&lt;&gt;L103,I103&lt;&gt;J103)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N103" t="s">
@@ -9929,7 +9948,7 @@
         <v>872</v>
       </c>
       <c r="M104" t="b">
-        <f>OR(K104&lt;&gt;L104,I104&lt;&gt;J104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N104" t="s">
@@ -9962,7 +9981,7 @@
         <v>874</v>
       </c>
       <c r="M105" t="b">
-        <f>OR(K105&lt;&gt;L105,I105&lt;&gt;J105)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N105" t="s">
@@ -9995,7 +10014,7 @@
         <v>876</v>
       </c>
       <c r="M106" t="b">
-        <f>OR(K106&lt;&gt;L106,I106&lt;&gt;J106)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N106" t="s">
@@ -10028,7 +10047,7 @@
         <v>878</v>
       </c>
       <c r="M107" t="b">
-        <f>OR(K107&lt;&gt;L107,I107&lt;&gt;J107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N107" t="s">
@@ -10061,7 +10080,7 @@
         <v>880</v>
       </c>
       <c r="M108" t="b">
-        <f>OR(K108&lt;&gt;L108,I108&lt;&gt;J108)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N108" t="s">
@@ -10094,7 +10113,7 @@
         <v>882</v>
       </c>
       <c r="M109" t="b">
-        <f>OR(K109&lt;&gt;L109,I109&lt;&gt;J109)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N109" t="s">
@@ -10127,7 +10146,7 @@
         <v>884</v>
       </c>
       <c r="M110" t="b">
-        <f>OR(K110&lt;&gt;L110,I110&lt;&gt;J110)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N110" t="s">
@@ -10160,7 +10179,7 @@
         <v>886</v>
       </c>
       <c r="M111" t="b">
-        <f>OR(K111&lt;&gt;L111,I111&lt;&gt;J111)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N111" t="s">
@@ -10193,7 +10212,7 @@
         <v>888</v>
       </c>
       <c r="M112" t="b">
-        <f>OR(K112&lt;&gt;L112,I112&lt;&gt;J112)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N112" t="s">
@@ -10226,7 +10245,7 @@
         <v>890</v>
       </c>
       <c r="M113" t="b">
-        <f>OR(K113&lt;&gt;L113,I113&lt;&gt;J113)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N113" t="s">
@@ -10259,7 +10278,7 @@
         <v>892</v>
       </c>
       <c r="M114" t="b">
-        <f>OR(K114&lt;&gt;L114,I114&lt;&gt;J114)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N114" t="s">
@@ -10292,7 +10311,7 @@
         <v>894</v>
       </c>
       <c r="M115" t="b">
-        <f>OR(K115&lt;&gt;L115,I115&lt;&gt;J115)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N115" t="s">
@@ -10325,7 +10344,7 @@
         <v>896</v>
       </c>
       <c r="M116" t="b">
-        <f>OR(K116&lt;&gt;L116,I116&lt;&gt;J116)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N116" t="s">
@@ -10358,7 +10377,7 @@
         <v>898</v>
       </c>
       <c r="M117" t="b">
-        <f>OR(K117&lt;&gt;L117,I117&lt;&gt;J117)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N117" t="s">
@@ -10391,7 +10410,7 @@
         <v>900</v>
       </c>
       <c r="M118" t="b">
-        <f>OR(K118&lt;&gt;L118,I118&lt;&gt;J118)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N118" t="s">
@@ -10424,7 +10443,7 @@
         <v>902</v>
       </c>
       <c r="M119" t="b">
-        <f>OR(K119&lt;&gt;L119,I119&lt;&gt;J119)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N119" t="s">
@@ -10457,7 +10476,7 @@
         <v>904</v>
       </c>
       <c r="M120" t="b">
-        <f>OR(K120&lt;&gt;L120,I120&lt;&gt;J120)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N120" t="s">
@@ -10490,7 +10509,7 @@
         <v>906</v>
       </c>
       <c r="M121" t="b">
-        <f>OR(K121&lt;&gt;L121,I121&lt;&gt;J121)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N121" t="s">
@@ -10523,7 +10542,7 @@
         <v>908</v>
       </c>
       <c r="M122" t="b">
-        <f>OR(K122&lt;&gt;L122,I122&lt;&gt;J122)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N122" t="s">
@@ -10556,7 +10575,7 @@
         <v>912</v>
       </c>
       <c r="M123" t="b">
-        <f>OR(K123&lt;&gt;L123,I123&lt;&gt;J123)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N123" t="s">
@@ -10582,14 +10601,14 @@
       <c r="J124" t="s">
         <v>830</v>
       </c>
-      <c r="K124" s="46" t="s">
+      <c r="K124" s="45" t="s">
         <v>1666</v>
       </c>
       <c r="L124" t="s">
         <v>910</v>
       </c>
       <c r="M124" t="b">
-        <f>OR(K124&lt;&gt;L124,I124&lt;&gt;J124)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N124" t="s">
@@ -10622,7 +10641,7 @@
         <v>953</v>
       </c>
       <c r="M125" t="b">
-        <f>OR(K125&lt;&gt;L125,I125&lt;&gt;J125)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N125" t="s">
@@ -10655,7 +10674,7 @@
         <v>955</v>
       </c>
       <c r="M126" t="b">
-        <f>OR(K126&lt;&gt;L126,I126&lt;&gt;J126)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N126" t="s">
@@ -10688,7 +10707,7 @@
         <v>1026</v>
       </c>
       <c r="M127" t="b">
-        <f>OR(K127&lt;&gt;L127,I127&lt;&gt;J127)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N127" t="s">
@@ -10721,7 +10740,7 @@
         <v>1061</v>
       </c>
       <c r="M128" t="b">
-        <f>OR(K128&lt;&gt;L128,I128&lt;&gt;J128)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N128" t="s">
@@ -10754,7 +10773,7 @@
         <v>1063</v>
       </c>
       <c r="M129" t="b">
-        <f>OR(K129&lt;&gt;L129,I129&lt;&gt;J129)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N129" t="s">
@@ -10787,7 +10806,7 @@
         <v>1065</v>
       </c>
       <c r="M130" t="b">
-        <f>OR(K130&lt;&gt;L130,I130&lt;&gt;J130)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N130" t="s">
@@ -10820,7 +10839,7 @@
         <v>1067</v>
       </c>
       <c r="M131" t="b">
-        <f>OR(K131&lt;&gt;L131,I131&lt;&gt;J131)</f>
+        <f t="shared" ref="M131:M194" si="2">OR(K131&lt;&gt;L131,I131&lt;&gt;J131)</f>
         <v>0</v>
       </c>
       <c r="N131" t="s">
@@ -10853,7 +10872,7 @@
         <v>1069</v>
       </c>
       <c r="M132" t="b">
-        <f>OR(K132&lt;&gt;L132,I132&lt;&gt;J132)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N132" t="s">
@@ -10879,14 +10898,14 @@
       <c r="J133" t="s">
         <v>1049</v>
       </c>
-      <c r="K133" s="46" t="s">
+      <c r="K133" s="45" t="s">
         <v>1679</v>
       </c>
       <c r="L133" t="s">
         <v>1071</v>
       </c>
       <c r="M133" t="b">
-        <f>OR(K133&lt;&gt;L133,I133&lt;&gt;J133)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N133" t="s">
@@ -10922,7 +10941,7 @@
         <v>1073</v>
       </c>
       <c r="M134" t="b">
-        <f>OR(K134&lt;&gt;L134,I134&lt;&gt;J134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N134" t="s">
@@ -10955,7 +10974,7 @@
         <v>1075</v>
       </c>
       <c r="M135" t="b">
-        <f>OR(K135&lt;&gt;L135,I135&lt;&gt;J135)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N135" t="s">
@@ -10988,7 +11007,7 @@
         <v>809</v>
       </c>
       <c r="M136" t="b">
-        <f>OR(K136&lt;&gt;L136,I136&lt;&gt;J136)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N136" t="s">
@@ -11021,7 +11040,7 @@
         <v>812</v>
       </c>
       <c r="M137" t="b">
-        <f>OR(K137&lt;&gt;L137,I137&lt;&gt;J137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N137" t="s">
@@ -11054,7 +11073,7 @@
         <v>814</v>
       </c>
       <c r="M138" t="b">
-        <f>OR(K138&lt;&gt;L138,I138&lt;&gt;J138)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N138" t="s">
@@ -11087,7 +11106,7 @@
         <v>1210</v>
       </c>
       <c r="M139" t="b">
-        <f>OR(K139&lt;&gt;L139,I139&lt;&gt;J139)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N139" t="s">
@@ -11120,7 +11139,7 @@
         <v>1212</v>
       </c>
       <c r="M140" t="b">
-        <f>OR(K140&lt;&gt;L140,I140&lt;&gt;J140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N140" t="s">
@@ -11153,7 +11172,7 @@
         <v>1214</v>
       </c>
       <c r="M141" t="b">
-        <f>OR(K141&lt;&gt;L141,I141&lt;&gt;J141)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N141" t="s">
@@ -11186,7 +11205,7 @@
         <v>1216</v>
       </c>
       <c r="M142" t="b">
-        <f>OR(K142&lt;&gt;L142,I142&lt;&gt;J142)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N142" t="s">
@@ -11222,7 +11241,7 @@
         <v>1179</v>
       </c>
       <c r="M143" t="b">
-        <f>OR(K143&lt;&gt;L143,I143&lt;&gt;J143)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N143" t="s">
@@ -11255,7 +11274,7 @@
         <v>1183</v>
       </c>
       <c r="M144" t="b">
-        <f>OR(K144&lt;&gt;L144,I144&lt;&gt;J144)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N144" t="s">
@@ -11288,7 +11307,7 @@
         <v>1185</v>
       </c>
       <c r="M145" t="b">
-        <f>OR(K145&lt;&gt;L145,I145&lt;&gt;J145)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N145" t="s">
@@ -11321,7 +11340,7 @@
         <v>1188</v>
       </c>
       <c r="M146" t="b">
-        <f>OR(K146&lt;&gt;L146,I146&lt;&gt;J146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N146" t="s">
@@ -11354,7 +11373,7 @@
         <v>1190</v>
       </c>
       <c r="M147" t="b">
-        <f>OR(K147&lt;&gt;L147,I147&lt;&gt;J147)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N147" t="s">
@@ -11387,7 +11406,7 @@
         <v>1192</v>
       </c>
       <c r="M148" t="b">
-        <f>OR(K148&lt;&gt;L148,I148&lt;&gt;J148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N148" t="s">
@@ -11420,7 +11439,7 @@
         <v>1194</v>
       </c>
       <c r="M149" t="b">
-        <f>OR(K149&lt;&gt;L149,I149&lt;&gt;J149)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N149" t="s">
@@ -11453,7 +11472,7 @@
         <v>1196</v>
       </c>
       <c r="M150" t="b">
-        <f>OR(K150&lt;&gt;L150,I150&lt;&gt;J150)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N150" t="s">
@@ -11486,7 +11505,7 @@
         <v>1198</v>
       </c>
       <c r="M151" t="b">
-        <f>OR(K151&lt;&gt;L151,I151&lt;&gt;J151)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N151" t="s">
@@ -11519,7 +11538,7 @@
         <v>1200</v>
       </c>
       <c r="M152" t="b">
-        <f>OR(K152&lt;&gt;L152,I152&lt;&gt;J152)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N152" t="s">
@@ -11552,7 +11571,7 @@
         <v>1202</v>
       </c>
       <c r="M153" t="b">
-        <f>OR(K153&lt;&gt;L153,I153&lt;&gt;J153)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N153" t="s">
@@ -11585,7 +11604,7 @@
         <v>1206</v>
       </c>
       <c r="M154" t="b">
-        <f>OR(K154&lt;&gt;L154,I154&lt;&gt;J154)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N154" t="s">
@@ -11618,7 +11637,7 @@
         <v>1208</v>
       </c>
       <c r="M155" t="b">
-        <f>OR(K155&lt;&gt;L155,I155&lt;&gt;J155)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N155" t="s">
@@ -11651,7 +11670,7 @@
         <v>1243</v>
       </c>
       <c r="M156" t="b">
-        <f>OR(K156&lt;&gt;L156,I156&lt;&gt;J156)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N156" t="s">
@@ -11684,7 +11703,7 @@
         <v>1245</v>
       </c>
       <c r="M157" t="b">
-        <f>OR(K157&lt;&gt;L157,I157&lt;&gt;J157)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N157" t="s">
@@ -11717,7 +11736,7 @@
         <v>1247</v>
       </c>
       <c r="M158" t="b">
-        <f>OR(K158&lt;&gt;L158,I158&lt;&gt;J158)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N158" t="s">
@@ -11750,7 +11769,7 @@
         <v>1249</v>
       </c>
       <c r="M159" t="b">
-        <f>OR(K159&lt;&gt;L159,I159&lt;&gt;J159)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N159" t="s">
@@ -11783,7 +11802,7 @@
         <v>1142</v>
       </c>
       <c r="M160" t="b">
-        <f>OR(K160&lt;&gt;L160,I160&lt;&gt;J160)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N160" t="s">
@@ -11816,7 +11835,7 @@
         <v>1146</v>
       </c>
       <c r="M161" t="b">
-        <f>OR(K161&lt;&gt;L161,I161&lt;&gt;J161)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N161" t="s">
@@ -11849,7 +11868,7 @@
         <v>1148</v>
       </c>
       <c r="M162" t="b">
-        <f>OR(K162&lt;&gt;L162,I162&lt;&gt;J162)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N162" t="s">
@@ -11885,7 +11904,7 @@
         <v>1150</v>
       </c>
       <c r="M163" t="b">
-        <f>OR(K163&lt;&gt;L163,I163&lt;&gt;J163)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N163" t="s">
@@ -11918,7 +11937,7 @@
         <v>1144</v>
       </c>
       <c r="M164" t="b">
-        <f>OR(K164&lt;&gt;L164,I164&lt;&gt;J164)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N164" t="s">
@@ -11951,7 +11970,7 @@
         <v>1152</v>
       </c>
       <c r="M165" t="b">
-        <f>OR(K165&lt;&gt;L165,I165&lt;&gt;J165)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N165" t="s">
@@ -11984,7 +12003,7 @@
         <v>1154</v>
       </c>
       <c r="M166" t="b">
-        <f>OR(K166&lt;&gt;L166,I166&lt;&gt;J166)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N166" t="s">
@@ -12017,7 +12036,7 @@
         <v>1156</v>
       </c>
       <c r="M167" t="b">
-        <f>OR(K167&lt;&gt;L167,I167&lt;&gt;J167)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N167" t="s">
@@ -12050,7 +12069,7 @@
         <v>914</v>
       </c>
       <c r="M168" t="b">
-        <f>OR(K168&lt;&gt;L168,I168&lt;&gt;J168)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N168" t="s">
@@ -12083,7 +12102,7 @@
         <v>816</v>
       </c>
       <c r="M169" t="b">
-        <f>OR(K169&lt;&gt;L169,I169&lt;&gt;J169)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N169" t="s">
@@ -12116,7 +12135,7 @@
         <v>1218</v>
       </c>
       <c r="M170" t="b">
-        <f>OR(K170&lt;&gt;L170,I170&lt;&gt;J170)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N170" t="s">
@@ -12132,11 +12151,11 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="171" spans="8:18">
+    <row r="171" spans="8:18" ht="15">
       <c r="H171" t="s">
         <v>533</v>
       </c>
-      <c r="I171" s="45" t="s">
+      <c r="I171" s="44" t="s">
         <v>1647</v>
       </c>
       <c r="J171" t="s">
@@ -12149,7 +12168,7 @@
         <v>1158</v>
       </c>
       <c r="M171" t="b">
-        <f>OR(K171&lt;&gt;L171,I171&lt;&gt;J171)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N171" t="s">
@@ -12165,11 +12184,11 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="172" spans="8:18">
+    <row r="172" spans="8:18" ht="15">
       <c r="H172" t="s">
         <v>533</v>
       </c>
-      <c r="I172" s="45" t="s">
+      <c r="I172" s="44" t="s">
         <v>1647</v>
       </c>
       <c r="J172" t="s">
@@ -12182,7 +12201,7 @@
         <v>1160</v>
       </c>
       <c r="M172" t="b">
-        <f>OR(K172&lt;&gt;L172,I172&lt;&gt;J172)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N172" t="s">
@@ -12198,11 +12217,11 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="173" spans="8:18">
+    <row r="173" spans="8:18" ht="15">
       <c r="H173" t="s">
         <v>533</v>
       </c>
-      <c r="I173" s="45" t="s">
+      <c r="I173" s="44" t="s">
         <v>1647</v>
       </c>
       <c r="J173" t="s">
@@ -12215,7 +12234,7 @@
         <v>1162</v>
       </c>
       <c r="M173" t="b">
-        <f>OR(K173&lt;&gt;L173,I173&lt;&gt;J173)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N173" t="s">
@@ -12231,11 +12250,11 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="174" spans="8:18">
+    <row r="174" spans="8:18" ht="15">
       <c r="H174" t="s">
         <v>533</v>
       </c>
-      <c r="I174" s="45" t="s">
+      <c r="I174" s="44" t="s">
         <v>1647</v>
       </c>
       <c r="J174" t="s">
@@ -12248,7 +12267,7 @@
         <v>1164</v>
       </c>
       <c r="M174" t="b">
-        <f>OR(K174&lt;&gt;L174,I174&lt;&gt;J174)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N174" t="s">
@@ -12281,7 +12300,7 @@
         <v>639</v>
       </c>
       <c r="M175" t="b">
-        <f>OR(K175&lt;&gt;L175,I175&lt;&gt;J175)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N175" t="s">
@@ -12314,7 +12333,7 @@
         <v>643</v>
       </c>
       <c r="M176" t="b">
-        <f>OR(K176&lt;&gt;L176,I176&lt;&gt;J176)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N176" t="s">
@@ -12347,7 +12366,7 @@
         <v>645</v>
       </c>
       <c r="M177" t="b">
-        <f>OR(K177&lt;&gt;L177,I177&lt;&gt;J177)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N177" t="s">
@@ -12380,7 +12399,7 @@
         <v>711</v>
       </c>
       <c r="M178" t="b">
-        <f>OR(K178&lt;&gt;L178,I178&lt;&gt;J178)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N178" t="s">
@@ -12413,7 +12432,7 @@
         <v>714</v>
       </c>
       <c r="M179" t="b">
-        <f>OR(K179&lt;&gt;L179,I179&lt;&gt;J179)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N179" t="s">
@@ -12446,7 +12465,7 @@
         <v>716</v>
       </c>
       <c r="M180" t="b">
-        <f>OR(K180&lt;&gt;L180,I180&lt;&gt;J180)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N180" t="s">
@@ -12472,14 +12491,14 @@
       <c r="J181" t="s">
         <v>648</v>
       </c>
-      <c r="K181" s="46" t="s">
+      <c r="K181" s="45" t="s">
         <v>1661</v>
       </c>
       <c r="L181" t="s">
         <v>671</v>
       </c>
       <c r="M181" t="b">
-        <f>OR(K181&lt;&gt;L181,I181&lt;&gt;J181)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N181" t="s">
@@ -12515,7 +12534,7 @@
         <v>649</v>
       </c>
       <c r="M182" t="b">
-        <f>OR(K182&lt;&gt;L182,I182&lt;&gt;J182)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N182" t="s">
@@ -12548,7 +12567,7 @@
         <v>651</v>
       </c>
       <c r="M183" t="b">
-        <f>OR(K183&lt;&gt;L183,I183&lt;&gt;J183)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N183" t="s">
@@ -12581,7 +12600,7 @@
         <v>675</v>
       </c>
       <c r="M184" t="b">
-        <f>OR(K184&lt;&gt;L184,I184&lt;&gt;J184)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N184" t="s">
@@ -12614,7 +12633,7 @@
         <v>653</v>
       </c>
       <c r="M185" t="b">
-        <f>OR(K185&lt;&gt;L185,I185&lt;&gt;J185)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N185" t="s">
@@ -12647,7 +12666,7 @@
         <v>677</v>
       </c>
       <c r="M186" t="b">
-        <f>OR(K186&lt;&gt;L186,I186&lt;&gt;J186)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N186" t="s">
@@ -12680,7 +12699,7 @@
         <v>655</v>
       </c>
       <c r="M187" t="b">
-        <f>OR(K187&lt;&gt;L187,I187&lt;&gt;J187)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N187" t="s">
@@ -12713,7 +12732,7 @@
         <v>661</v>
       </c>
       <c r="M188" t="b">
-        <f>OR(K188&lt;&gt;L188,I188&lt;&gt;J188)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N188" t="s">
@@ -12749,7 +12768,7 @@
         <v>681</v>
       </c>
       <c r="M189" t="b">
-        <f>OR(K189&lt;&gt;L189,I189&lt;&gt;J189)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N189" t="s">
@@ -12782,7 +12801,7 @@
         <v>683</v>
       </c>
       <c r="M190" t="b">
-        <f>OR(K190&lt;&gt;L190,I190&lt;&gt;J190)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N190" t="s">
@@ -12815,7 +12834,7 @@
         <v>685</v>
       </c>
       <c r="M191" t="b">
-        <f>OR(K191&lt;&gt;L191,I191&lt;&gt;J191)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N191" t="s">
@@ -12848,7 +12867,7 @@
         <v>657</v>
       </c>
       <c r="M192" t="b">
-        <f>OR(K192&lt;&gt;L192,I192&lt;&gt;J192)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N192" t="s">
@@ -12881,7 +12900,7 @@
         <v>659</v>
       </c>
       <c r="M193" t="b">
-        <f>OR(K193&lt;&gt;L193,I193&lt;&gt;J193)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N193" t="s">
@@ -12914,7 +12933,7 @@
         <v>687</v>
       </c>
       <c r="M194" t="b">
-        <f>OR(K194&lt;&gt;L194,I194&lt;&gt;J194)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N194" t="s">
@@ -12947,7 +12966,7 @@
         <v>689</v>
       </c>
       <c r="M195" t="b">
-        <f>OR(K195&lt;&gt;L195,I195&lt;&gt;J195)</f>
+        <f t="shared" ref="M195:M258" si="3">OR(K195&lt;&gt;L195,I195&lt;&gt;J195)</f>
         <v>0</v>
       </c>
       <c r="N195" t="s">
@@ -12980,7 +12999,7 @@
         <v>691</v>
       </c>
       <c r="M196" t="b">
-        <f>OR(K196&lt;&gt;L196,I196&lt;&gt;J196)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N196" t="s">
@@ -13013,7 +13032,7 @@
         <v>701</v>
       </c>
       <c r="M197" t="b">
-        <f>OR(K197&lt;&gt;L197,I197&lt;&gt;J197)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N197" t="s">
@@ -13046,7 +13065,7 @@
         <v>679</v>
       </c>
       <c r="M198" t="b">
-        <f>OR(K198&lt;&gt;L198,I198&lt;&gt;J198)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N198" t="s">
@@ -13079,7 +13098,7 @@
         <v>663</v>
       </c>
       <c r="M199" t="b">
-        <f>OR(K199&lt;&gt;L199,I199&lt;&gt;J199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N199" t="s">
@@ -13112,7 +13131,7 @@
         <v>673</v>
       </c>
       <c r="M200" t="b">
-        <f>OR(K200&lt;&gt;L200,I200&lt;&gt;J200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N200" t="s">
@@ -13145,7 +13164,7 @@
         <v>693</v>
       </c>
       <c r="M201" t="b">
-        <f>OR(K201&lt;&gt;L201,I201&lt;&gt;J201)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N201" t="s">
@@ -13178,7 +13197,7 @@
         <v>695</v>
       </c>
       <c r="M202" t="b">
-        <f>OR(K202&lt;&gt;L202,I202&lt;&gt;J202)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N202" t="s">
@@ -13211,7 +13230,7 @@
         <v>665</v>
       </c>
       <c r="M203" t="b">
-        <f>OR(K203&lt;&gt;L203,I203&lt;&gt;J203)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N203" t="s">
@@ -13244,7 +13263,7 @@
         <v>703</v>
       </c>
       <c r="M204" t="b">
-        <f>OR(K204&lt;&gt;L204,I204&lt;&gt;J204)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N204" t="s">
@@ -13277,7 +13296,7 @@
         <v>705</v>
       </c>
       <c r="M205" t="b">
-        <f>OR(K205&lt;&gt;L205,I205&lt;&gt;J205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N205" t="s">
@@ -13310,7 +13329,7 @@
         <v>697</v>
       </c>
       <c r="M206" t="b">
-        <f>OR(K206&lt;&gt;L206,I206&lt;&gt;J206)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N206" t="s">
@@ -13343,7 +13362,7 @@
         <v>667</v>
       </c>
       <c r="M207" t="b">
-        <f>OR(K207&lt;&gt;L207,I207&lt;&gt;J207)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N207" t="s">
@@ -13376,7 +13395,7 @@
         <v>707</v>
       </c>
       <c r="M208" t="b">
-        <f>OR(K208&lt;&gt;L208,I208&lt;&gt;J208)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N208" t="s">
@@ -13409,7 +13428,7 @@
         <v>699</v>
       </c>
       <c r="M209" t="b">
-        <f>OR(K209&lt;&gt;L209,I209&lt;&gt;J209)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N209" t="s">
@@ -13442,7 +13461,7 @@
         <v>669</v>
       </c>
       <c r="M210" t="b">
-        <f>OR(K210&lt;&gt;L210,I210&lt;&gt;J210)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N210" t="s">
@@ -13475,7 +13494,7 @@
         <v>1043</v>
       </c>
       <c r="M211" t="b">
-        <f>OR(K211&lt;&gt;L211,I211&lt;&gt;J211)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N211" t="s">
@@ -13508,7 +13527,7 @@
         <v>1046</v>
       </c>
       <c r="M212" t="b">
-        <f>OR(K212&lt;&gt;L212,I212&lt;&gt;J212)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N212" t="s">
@@ -13541,7 +13560,7 @@
         <v>552</v>
       </c>
       <c r="M213" t="b">
-        <f>OR(K213&lt;&gt;L213,I213&lt;&gt;J213)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N213" t="s">
@@ -13574,7 +13593,7 @@
         <v>554</v>
       </c>
       <c r="M214" t="b">
-        <f>OR(K214&lt;&gt;L214,I214&lt;&gt;J214)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N214" t="s">
@@ -13607,7 +13626,7 @@
         <v>557</v>
       </c>
       <c r="M215" t="b">
-        <f>OR(K215&lt;&gt;L215,I215&lt;&gt;J215)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N215" t="s">
@@ -13640,7 +13659,7 @@
         <v>559</v>
       </c>
       <c r="M216" t="b">
-        <f>OR(K216&lt;&gt;L216,I216&lt;&gt;J216)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N216" t="s">
@@ -13673,7 +13692,7 @@
         <v>561</v>
       </c>
       <c r="M217" t="b">
-        <f>OR(K217&lt;&gt;L217,I217&lt;&gt;J217)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N217" t="s">
@@ -13706,7 +13725,7 @@
         <v>563</v>
       </c>
       <c r="M218" t="b">
-        <f>OR(K218&lt;&gt;L218,I218&lt;&gt;J218)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N218" t="s">
@@ -13739,7 +13758,7 @@
         <v>1107</v>
       </c>
       <c r="M219" t="b">
-        <f>OR(K219&lt;&gt;L219,I219&lt;&gt;J219)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N219" t="s">
@@ -13772,7 +13791,7 @@
         <v>1109</v>
       </c>
       <c r="M220" t="b">
-        <f>OR(K220&lt;&gt;L220,I220&lt;&gt;J220)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N220" t="s">
@@ -13805,7 +13824,7 @@
         <v>1111</v>
       </c>
       <c r="M221" t="b">
-        <f>OR(K221&lt;&gt;L221,I221&lt;&gt;J221)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N221" t="s">
@@ -13838,7 +13857,7 @@
         <v>1113</v>
       </c>
       <c r="M222" t="b">
-        <f>OR(K222&lt;&gt;L222,I222&lt;&gt;J222)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N222" t="s">
@@ -13871,7 +13890,7 @@
         <v>1077</v>
       </c>
       <c r="M223" t="b">
-        <f>OR(K223&lt;&gt;L223,I223&lt;&gt;J223)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N223" t="s">
@@ -13904,7 +13923,7 @@
         <v>957</v>
       </c>
       <c r="M224" t="b">
-        <f>OR(K224&lt;&gt;L224,I224&lt;&gt;J224)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N224" t="s">
@@ -13937,7 +13956,7 @@
         <v>959</v>
       </c>
       <c r="M225" t="b">
-        <f>OR(K225&lt;&gt;L225,I225&lt;&gt;J225)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N225" t="s">
@@ -13970,7 +13989,7 @@
         <v>961</v>
       </c>
       <c r="M226" t="b">
-        <f>OR(K226&lt;&gt;L226,I226&lt;&gt;J226)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N226" t="s">
@@ -14003,7 +14022,7 @@
         <v>963</v>
       </c>
       <c r="M227" t="b">
-        <f>OR(K227&lt;&gt;L227,I227&lt;&gt;J227)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N227" t="s">
@@ -14036,7 +14055,7 @@
         <v>965</v>
       </c>
       <c r="M228" t="b">
-        <f>OR(K228&lt;&gt;L228,I228&lt;&gt;J228)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N228" t="s">
@@ -14069,7 +14088,7 @@
         <v>730</v>
       </c>
       <c r="M229" t="b">
-        <f>OR(K229&lt;&gt;L229,I229&lt;&gt;J229)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N229" t="s">
@@ -14102,7 +14121,7 @@
         <v>733</v>
       </c>
       <c r="M230" t="b">
-        <f>OR(K230&lt;&gt;L230,I230&lt;&gt;J230)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N230" t="s">
@@ -14135,7 +14154,7 @@
         <v>735</v>
       </c>
       <c r="M231" t="b">
-        <f>OR(K231&lt;&gt;L231,I231&lt;&gt;J231)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N231" t="s">
@@ -14168,7 +14187,7 @@
         <v>737</v>
       </c>
       <c r="M232" t="b">
-        <f>OR(K232&lt;&gt;L232,I232&lt;&gt;J232)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N232" t="s">
@@ -14201,7 +14220,7 @@
         <v>739</v>
       </c>
       <c r="M233" t="b">
-        <f>OR(K233&lt;&gt;L233,I233&lt;&gt;J233)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N233" t="s">
@@ -14234,7 +14253,7 @@
         <v>741</v>
       </c>
       <c r="M234" t="b">
-        <f>OR(K234&lt;&gt;L234,I234&lt;&gt;J234)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N234" t="s">
@@ -14267,7 +14286,7 @@
         <v>743</v>
       </c>
       <c r="M235" t="b">
-        <f>OR(K235&lt;&gt;L235,I235&lt;&gt;J235)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N235" t="s">
@@ -14300,7 +14319,7 @@
         <v>745</v>
       </c>
       <c r="M236" t="b">
-        <f>OR(K236&lt;&gt;L236,I236&lt;&gt;J236)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N236" t="s">
@@ -14333,7 +14352,7 @@
         <v>747</v>
       </c>
       <c r="M237" t="b">
-        <f>OR(K237&lt;&gt;L237,I237&lt;&gt;J237)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N237" t="s">
@@ -14366,7 +14385,7 @@
         <v>749</v>
       </c>
       <c r="M238" t="b">
-        <f>OR(K238&lt;&gt;L238,I238&lt;&gt;J238)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N238" t="s">
@@ -14399,7 +14418,7 @@
         <v>751</v>
       </c>
       <c r="M239" t="b">
-        <f>OR(K239&lt;&gt;L239,I239&lt;&gt;J239)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N239" t="s">
@@ -14432,7 +14451,7 @@
         <v>753</v>
       </c>
       <c r="M240" t="b">
-        <f>OR(K240&lt;&gt;L240,I240&lt;&gt;J240)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N240" t="s">
@@ -14465,7 +14484,7 @@
         <v>756</v>
       </c>
       <c r="M241" t="b">
-        <f>OR(K241&lt;&gt;L241,I241&lt;&gt;J241)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N241" t="s">
@@ -14498,7 +14517,7 @@
         <v>758</v>
       </c>
       <c r="M242" t="b">
-        <f>OR(K242&lt;&gt;L242,I242&lt;&gt;J242)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N242" t="s">
@@ -14531,7 +14550,7 @@
         <v>760</v>
       </c>
       <c r="M243" t="b">
-        <f>OR(K243&lt;&gt;L243,I243&lt;&gt;J243)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N243" t="s">
@@ -14564,7 +14583,7 @@
         <v>762</v>
       </c>
       <c r="M244" t="b">
-        <f>OR(K244&lt;&gt;L244,I244&lt;&gt;J244)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N244" t="s">
@@ -14597,7 +14616,7 @@
         <v>764</v>
       </c>
       <c r="M245" t="b">
-        <f>OR(K245&lt;&gt;L245,I245&lt;&gt;J245)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N245" t="s">
@@ -14630,7 +14649,7 @@
         <v>766</v>
       </c>
       <c r="M246" t="b">
-        <f>OR(K246&lt;&gt;L246,I246&lt;&gt;J246)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N246" t="s">
@@ -14663,7 +14682,7 @@
         <v>770</v>
       </c>
       <c r="M247" t="b">
-        <f>OR(K247&lt;&gt;L247,I247&lt;&gt;J247)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N247" t="s">
@@ -14696,7 +14715,7 @@
         <v>772</v>
       </c>
       <c r="M248" t="b">
-        <f>OR(K248&lt;&gt;L248,I248&lt;&gt;J248)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N248" t="s">
@@ -14729,7 +14748,7 @@
         <v>774</v>
       </c>
       <c r="M249" t="b">
-        <f>OR(K249&lt;&gt;L249,I249&lt;&gt;J249)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N249" t="s">
@@ -14762,7 +14781,7 @@
         <v>776</v>
       </c>
       <c r="M250" t="b">
-        <f>OR(K250&lt;&gt;L250,I250&lt;&gt;J250)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N250" t="s">
@@ -14795,7 +14814,7 @@
         <v>778</v>
       </c>
       <c r="M251" t="b">
-        <f>OR(K251&lt;&gt;L251,I251&lt;&gt;J251)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N251" t="s">
@@ -14828,7 +14847,7 @@
         <v>780</v>
       </c>
       <c r="M252" t="b">
-        <f>OR(K252&lt;&gt;L252,I252&lt;&gt;J252)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N252" t="s">
@@ -14861,7 +14880,7 @@
         <v>782</v>
       </c>
       <c r="M253" t="b">
-        <f>OR(K253&lt;&gt;L253,I253&lt;&gt;J253)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N253" t="s">
@@ -14894,7 +14913,7 @@
         <v>784</v>
       </c>
       <c r="M254" t="b">
-        <f>OR(K254&lt;&gt;L254,I254&lt;&gt;J254)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N254" t="s">
@@ -14920,14 +14939,14 @@
       <c r="J255" t="s">
         <v>729</v>
       </c>
-      <c r="K255" s="46" t="s">
+      <c r="K255" s="45" t="s">
         <v>1664</v>
       </c>
       <c r="L255" t="s">
         <v>768</v>
       </c>
       <c r="M255" t="b">
-        <f>OR(K255&lt;&gt;L255,I255&lt;&gt;J255)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N255" t="s">
@@ -14963,7 +14982,7 @@
         <v>786</v>
       </c>
       <c r="M256" t="b">
-        <f>OR(K256&lt;&gt;L256,I256&lt;&gt;J256)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N256" t="s">
@@ -14996,7 +15015,7 @@
         <v>788</v>
       </c>
       <c r="M257" t="b">
-        <f>OR(K257&lt;&gt;L257,I257&lt;&gt;J257)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N257" t="s">
@@ -15029,7 +15048,7 @@
         <v>790</v>
       </c>
       <c r="M258" t="b">
-        <f>OR(K258&lt;&gt;L258,I258&lt;&gt;J258)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N258" t="s">
@@ -15062,7 +15081,7 @@
         <v>792</v>
       </c>
       <c r="M259" t="b">
-        <f>OR(K259&lt;&gt;L259,I259&lt;&gt;J259)</f>
+        <f t="shared" ref="M259:M322" si="4">OR(K259&lt;&gt;L259,I259&lt;&gt;J259)</f>
         <v>0</v>
       </c>
       <c r="N259" t="s">
@@ -15095,7 +15114,7 @@
         <v>794</v>
       </c>
       <c r="M260" t="b">
-        <f>OR(K260&lt;&gt;L260,I260&lt;&gt;J260)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N260" t="s">
@@ -15128,7 +15147,7 @@
         <v>796</v>
       </c>
       <c r="M261" t="b">
-        <f>OR(K261&lt;&gt;L261,I261&lt;&gt;J261)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N261" t="s">
@@ -15161,7 +15180,7 @@
         <v>798</v>
       </c>
       <c r="M262" t="b">
-        <f>OR(K262&lt;&gt;L262,I262&lt;&gt;J262)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N262" t="s">
@@ -15194,7 +15213,7 @@
         <v>800</v>
       </c>
       <c r="M263" t="b">
-        <f>OR(K263&lt;&gt;L263,I263&lt;&gt;J263)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N263" t="s">
@@ -15227,7 +15246,7 @@
         <v>802</v>
       </c>
       <c r="M264" t="b">
-        <f>OR(K264&lt;&gt;L264,I264&lt;&gt;J264)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N264" t="s">
@@ -15260,7 +15279,7 @@
         <v>804</v>
       </c>
       <c r="M265" t="b">
-        <f>OR(K265&lt;&gt;L265,I265&lt;&gt;J265)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N265" t="s">
@@ -15293,7 +15312,7 @@
         <v>806</v>
       </c>
       <c r="M266" t="b">
-        <f>OR(K266&lt;&gt;L266,I266&lt;&gt;J266)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N266" t="s">
@@ -15326,7 +15345,7 @@
         <v>621</v>
       </c>
       <c r="M267" t="b">
-        <f>OR(K267&lt;&gt;L267,I267&lt;&gt;J267)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N267" t="s">
@@ -15359,7 +15378,7 @@
         <v>967</v>
       </c>
       <c r="M268" t="b">
-        <f>OR(K268&lt;&gt;L268,I268&lt;&gt;J268)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N268" t="s">
@@ -15392,7 +15411,7 @@
         <v>969</v>
       </c>
       <c r="M269" t="b">
-        <f>OR(K269&lt;&gt;L269,I269&lt;&gt;J269)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N269" t="s">
@@ -15425,7 +15444,7 @@
         <v>973</v>
       </c>
       <c r="M270" t="b">
-        <f>OR(K270&lt;&gt;L270,I270&lt;&gt;J270)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N270" t="s">
@@ -15461,7 +15480,7 @@
         <v>975</v>
       </c>
       <c r="M271" t="b">
-        <f>OR(K271&lt;&gt;L271,I271&lt;&gt;J271)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N271" t="s">
@@ -15497,7 +15516,7 @@
         <v>926</v>
       </c>
       <c r="M272" t="b">
-        <f>OR(K272&lt;&gt;L272,I272&lt;&gt;J272)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N272" t="s">
@@ -15530,7 +15549,7 @@
         <v>929</v>
       </c>
       <c r="M273" t="b">
-        <f>OR(K273&lt;&gt;L273,I273&lt;&gt;J273)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N273" t="s">
@@ -15563,7 +15582,7 @@
         <v>931</v>
       </c>
       <c r="M274" t="b">
-        <f>OR(K274&lt;&gt;L274,I274&lt;&gt;J274)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N274" t="s">
@@ -15596,7 +15615,7 @@
         <v>977</v>
       </c>
       <c r="M275" t="b">
-        <f>OR(K275&lt;&gt;L275,I275&lt;&gt;J275)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N275" t="s">
@@ -15629,7 +15648,7 @@
         <v>979</v>
       </c>
       <c r="M276" t="b">
-        <f>OR(K276&lt;&gt;L276,I276&lt;&gt;J276)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N276" t="s">
@@ -15662,7 +15681,7 @@
         <v>933</v>
       </c>
       <c r="M277" t="b">
-        <f>OR(K277&lt;&gt;L277,I277&lt;&gt;J277)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N277" t="s">
@@ -15695,7 +15714,7 @@
         <v>935</v>
       </c>
       <c r="M278" t="b">
-        <f>OR(K278&lt;&gt;L278,I278&lt;&gt;J278)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N278" t="s">
@@ -15728,7 +15747,7 @@
         <v>981</v>
       </c>
       <c r="M279" t="b">
-        <f>OR(K279&lt;&gt;L279,I279&lt;&gt;J279)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N279" t="s">
@@ -15761,7 +15780,7 @@
         <v>983</v>
       </c>
       <c r="M280" t="b">
-        <f>OR(K280&lt;&gt;L280,I280&lt;&gt;J280)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N280" t="s">
@@ -15794,7 +15813,7 @@
         <v>971</v>
       </c>
       <c r="M281" t="b">
-        <f>OR(K281&lt;&gt;L281,I281&lt;&gt;J281)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N281" t="s">
@@ -15830,7 +15849,7 @@
         <v>985</v>
       </c>
       <c r="M282" t="b">
-        <f>OR(K282&lt;&gt;L282,I282&lt;&gt;J282)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N282" t="s">
@@ -15863,7 +15882,7 @@
         <v>987</v>
       </c>
       <c r="M283" t="b">
-        <f>OR(K283&lt;&gt;L283,I283&lt;&gt;J283)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N283" t="s">
@@ -15896,7 +15915,7 @@
         <v>989</v>
       </c>
       <c r="M284" t="b">
-        <f>OR(K284&lt;&gt;L284,I284&lt;&gt;J284)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N284" t="s">
@@ -15922,14 +15941,14 @@
       <c r="J285" t="s">
         <v>729</v>
       </c>
-      <c r="K285" s="46" t="s">
+      <c r="K285" s="45" t="s">
         <v>1683</v>
       </c>
       <c r="L285" t="s">
         <v>991</v>
       </c>
       <c r="M285" t="b">
-        <f>OR(K285&lt;&gt;L285,I285&lt;&gt;J285)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N285" t="s">
@@ -15962,7 +15981,7 @@
         <v>993</v>
       </c>
       <c r="M286" t="b">
-        <f>OR(K286&lt;&gt;L286,I286&lt;&gt;J286)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N286" t="s">
@@ -15995,7 +16014,7 @@
         <v>937</v>
       </c>
       <c r="M287" t="b">
-        <f>OR(K287&lt;&gt;L287,I287&lt;&gt;J287)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N287" t="s">
@@ -16028,7 +16047,7 @@
         <v>995</v>
       </c>
       <c r="M288" t="b">
-        <f>OR(K288&lt;&gt;L288,I288&lt;&gt;J288)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N288" t="s">
@@ -16061,7 +16080,7 @@
         <v>997</v>
       </c>
       <c r="M289" t="b">
-        <f>OR(K289&lt;&gt;L289,I289&lt;&gt;J289)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N289" t="s">
@@ -16094,7 +16113,7 @@
         <v>999</v>
       </c>
       <c r="M290" t="b">
-        <f>OR(K290&lt;&gt;L290,I290&lt;&gt;J290)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N290" t="s">
@@ -16130,7 +16149,7 @@
         <v>939</v>
       </c>
       <c r="M291" t="b">
-        <f>OR(K291&lt;&gt;L291,I291&lt;&gt;J291)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N291" t="s">
@@ -16163,7 +16182,7 @@
         <v>1001</v>
       </c>
       <c r="M292" t="b">
-        <f>OR(K292&lt;&gt;L292,I292&lt;&gt;J292)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N292" t="s">
@@ -16179,7 +16198,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="293" spans="8:18" ht="15">
+    <row r="293" spans="8:18">
       <c r="H293" t="s">
         <v>1003</v>
       </c>
@@ -16196,7 +16215,7 @@
         <v>1028</v>
       </c>
       <c r="M293" t="b">
-        <f>OR(K293&lt;&gt;L293,I293&lt;&gt;J293)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N293" t="s">
@@ -16212,7 +16231,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="294" spans="8:18" ht="15">
+    <row r="294" spans="8:18">
       <c r="H294" t="s">
         <v>1003</v>
       </c>
@@ -16229,7 +16248,7 @@
         <v>1030</v>
       </c>
       <c r="M294" t="b">
-        <f>OR(K294&lt;&gt;L294,I294&lt;&gt;J294)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N294" t="s">
@@ -16245,7 +16264,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="295" spans="8:18" ht="15">
+    <row r="295" spans="8:18">
       <c r="H295" t="s">
         <v>1003</v>
       </c>
@@ -16262,7 +16281,7 @@
         <v>1032</v>
       </c>
       <c r="M295" t="b">
-        <f>OR(K295&lt;&gt;L295,I295&lt;&gt;J295)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N295" t="s">
@@ -16278,7 +16297,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="296" spans="8:18" ht="15">
+    <row r="296" spans="8:18">
       <c r="H296" t="s">
         <v>586</v>
       </c>
@@ -16295,7 +16314,7 @@
         <v>916</v>
       </c>
       <c r="M296" t="b">
-        <f>OR(K296&lt;&gt;L296,I296&lt;&gt;J296)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N296" t="s">
@@ -16328,7 +16347,7 @@
         <v>918</v>
       </c>
       <c r="M297" t="b">
-        <f>OR(K297&lt;&gt;L297,I297&lt;&gt;J297)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N297" t="s">
@@ -16361,7 +16380,7 @@
         <v>920</v>
       </c>
       <c r="M298" t="b">
-        <f>OR(K298&lt;&gt;L298,I298&lt;&gt;J298)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N298" t="s">
@@ -16394,7 +16413,7 @@
         <v>922</v>
       </c>
       <c r="M299" t="b">
-        <f>OR(K299&lt;&gt;L299,I299&lt;&gt;J299)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N299" t="s">
@@ -16430,7 +16449,7 @@
         <v>1079</v>
       </c>
       <c r="M300" t="b">
-        <f>OR(K300&lt;&gt;L300,I300&lt;&gt;J300)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N300" t="s">
@@ -16463,7 +16482,7 @@
         <v>1081</v>
       </c>
       <c r="M301" t="b">
-        <f>OR(K301&lt;&gt;L301,I301&lt;&gt;J301)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N301" t="s">
@@ -16496,7 +16515,7 @@
         <v>1083</v>
       </c>
       <c r="M302" t="b">
-        <f>OR(K302&lt;&gt;L302,I302&lt;&gt;J302)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N302" t="s">
@@ -16529,7 +16548,7 @@
         <v>1034</v>
       </c>
       <c r="M303" t="b">
-        <f>OR(K303&lt;&gt;L303,I303&lt;&gt;J303)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N303" t="s">
@@ -16562,7 +16581,7 @@
         <v>1036</v>
       </c>
       <c r="M304" t="b">
-        <f>OR(K304&lt;&gt;L304,I304&lt;&gt;J304)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N304" t="s">
@@ -16595,7 +16614,7 @@
         <v>1038</v>
       </c>
       <c r="M305" t="b">
-        <f>OR(K305&lt;&gt;L305,I305&lt;&gt;J305)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N305" t="s">
@@ -16628,7 +16647,7 @@
         <v>1040</v>
       </c>
       <c r="M306" t="b">
-        <f>OR(K306&lt;&gt;L306,I306&lt;&gt;J306)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N306" t="s">
@@ -16661,7 +16680,7 @@
         <v>1125</v>
       </c>
       <c r="M307" t="b">
-        <f>OR(K307&lt;&gt;L307,I307&lt;&gt;J307)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N307" t="s">
@@ -16694,7 +16713,7 @@
         <v>1127</v>
       </c>
       <c r="M308" t="b">
-        <f>OR(K308&lt;&gt;L308,I308&lt;&gt;J308)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N308" t="s">
@@ -16727,7 +16746,7 @@
         <v>1129</v>
       </c>
       <c r="M309" t="b">
-        <f>OR(K309&lt;&gt;L309,I309&lt;&gt;J309)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N309" t="s">
@@ -16760,7 +16779,7 @@
         <v>1289</v>
       </c>
       <c r="M310" t="b">
-        <f>OR(K310&lt;&gt;L310,I310&lt;&gt;J310)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N310" t="s">
@@ -16793,7 +16812,7 @@
         <v>1291</v>
       </c>
       <c r="M311" t="b">
-        <f>OR(K311&lt;&gt;L311,I311&lt;&gt;J311)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N311" t="s">
@@ -16826,7 +16845,7 @@
         <v>1293</v>
       </c>
       <c r="M312" t="b">
-        <f>OR(K312&lt;&gt;L312,I312&lt;&gt;J312)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N312" t="s">
@@ -16859,7 +16878,7 @@
         <v>1255</v>
       </c>
       <c r="M313" t="b">
-        <f>OR(K313&lt;&gt;L313,I313&lt;&gt;J313)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N313" t="s">
@@ -16892,7 +16911,7 @@
         <v>1295</v>
       </c>
       <c r="M314" t="b">
-        <f>OR(K314&lt;&gt;L314,I314&lt;&gt;J314)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N314" t="s">
@@ -16925,7 +16944,7 @@
         <v>1257</v>
       </c>
       <c r="M315" t="b">
-        <f>OR(K315&lt;&gt;L315,I315&lt;&gt;J315)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N315" t="s">
@@ -16958,7 +16977,7 @@
         <v>1259</v>
       </c>
       <c r="M316" t="b">
-        <f>OR(K316&lt;&gt;L316,I316&lt;&gt;J316)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N316" t="s">
@@ -16991,7 +17010,7 @@
         <v>1261</v>
       </c>
       <c r="M317" t="b">
-        <f>OR(K317&lt;&gt;L317,I317&lt;&gt;J317)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N317" t="s">
@@ -17024,7 +17043,7 @@
         <v>1297</v>
       </c>
       <c r="M318" t="b">
-        <f>OR(K318&lt;&gt;L318,I318&lt;&gt;J318)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N318" t="s">
@@ -17057,7 +17076,7 @@
         <v>1263</v>
       </c>
       <c r="M319" t="b">
-        <f>OR(K319&lt;&gt;L319,I319&lt;&gt;J319)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N319" t="s">
@@ -17090,7 +17109,7 @@
         <v>1265</v>
       </c>
       <c r="M320" t="b">
-        <f>OR(K320&lt;&gt;L320,I320&lt;&gt;J320)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N320" t="s">
@@ -17123,7 +17142,7 @@
         <v>1299</v>
       </c>
       <c r="M321" t="b">
-        <f>OR(K321&lt;&gt;L321,I321&lt;&gt;J321)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N321" t="s">
@@ -17156,7 +17175,7 @@
         <v>1267</v>
       </c>
       <c r="M322" t="b">
-        <f>OR(K322&lt;&gt;L322,I322&lt;&gt;J322)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N322" t="s">
@@ -17189,7 +17208,7 @@
         <v>1269</v>
       </c>
       <c r="M323" t="b">
-        <f>OR(K323&lt;&gt;L323,I323&lt;&gt;J323)</f>
+        <f t="shared" ref="M323:M361" si="5">OR(K323&lt;&gt;L323,I323&lt;&gt;J323)</f>
         <v>0</v>
       </c>
       <c r="N323" t="s">
@@ -17222,7 +17241,7 @@
         <v>1271</v>
       </c>
       <c r="M324" t="b">
-        <f>OR(K324&lt;&gt;L324,I324&lt;&gt;J324)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N324" t="s">
@@ -17255,7 +17274,7 @@
         <v>1273</v>
       </c>
       <c r="M325" t="b">
-        <f>OR(K325&lt;&gt;L325,I325&lt;&gt;J325)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N325" t="s">
@@ -17288,7 +17307,7 @@
         <v>1275</v>
       </c>
       <c r="M326" t="b">
-        <f>OR(K326&lt;&gt;L326,I326&lt;&gt;J326)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N326" t="s">
@@ -17321,7 +17340,7 @@
         <v>1277</v>
       </c>
       <c r="M327" t="b">
-        <f>OR(K327&lt;&gt;L327,I327&lt;&gt;J327)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N327" t="s">
@@ -17354,7 +17373,7 @@
         <v>1279</v>
       </c>
       <c r="M328" t="b">
-        <f>OR(K328&lt;&gt;L328,I328&lt;&gt;J328)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N328" t="s">
@@ -17387,7 +17406,7 @@
         <v>1281</v>
       </c>
       <c r="M329" t="b">
-        <f>OR(K329&lt;&gt;L329,I329&lt;&gt;J329)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N329" t="s">
@@ -17420,7 +17439,7 @@
         <v>1283</v>
       </c>
       <c r="M330" t="b">
-        <f>OR(K330&lt;&gt;L330,I330&lt;&gt;J330)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N330" t="s">
@@ -17453,7 +17472,7 @@
         <v>1285</v>
       </c>
       <c r="M331" t="b">
-        <f>OR(K331&lt;&gt;L331,I331&lt;&gt;J331)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N331" t="s">
@@ -17486,7 +17505,7 @@
         <v>1287</v>
       </c>
       <c r="M332" t="b">
-        <f>OR(K332&lt;&gt;L332,I332&lt;&gt;J332)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N332" t="s">
@@ -17519,7 +17538,7 @@
         <v>818</v>
       </c>
       <c r="M333" t="b">
-        <f>OR(K333&lt;&gt;L333,I333&lt;&gt;J333)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N333" t="s">
@@ -17552,7 +17571,7 @@
         <v>820</v>
       </c>
       <c r="M334" t="b">
-        <f>OR(K334&lt;&gt;L334,I334&lt;&gt;J334)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N334" t="s">
@@ -17585,7 +17604,7 @@
         <v>822</v>
       </c>
       <c r="M335" t="b">
-        <f>OR(K335&lt;&gt;L335,I335&lt;&gt;J335)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N335" t="s">
@@ -17618,7 +17637,7 @@
         <v>824</v>
       </c>
       <c r="M336" t="b">
-        <f>OR(K336&lt;&gt;L336,I336&lt;&gt;J336)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N336" t="s">
@@ -17651,7 +17670,7 @@
         <v>826</v>
       </c>
       <c r="M337" t="b">
-        <f>OR(K337&lt;&gt;L337,I337&lt;&gt;J337)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N337" t="s">
@@ -17684,7 +17703,7 @@
         <v>828</v>
       </c>
       <c r="M338" t="b">
-        <f>OR(K338&lt;&gt;L338,I338&lt;&gt;J338)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N338" t="s">
@@ -17717,7 +17736,7 @@
         <v>623</v>
       </c>
       <c r="M339" t="b">
-        <f>OR(K339&lt;&gt;L339,I339&lt;&gt;J339)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N339" t="s">
@@ -17750,7 +17769,7 @@
         <v>625</v>
       </c>
       <c r="M340" t="b">
-        <f>OR(K340&lt;&gt;L340,I340&lt;&gt;J340)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N340" t="s">
@@ -17783,7 +17802,7 @@
         <v>627</v>
       </c>
       <c r="M341" t="b">
-        <f>OR(K341&lt;&gt;L341,I341&lt;&gt;J341)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N341" t="s">
@@ -17816,7 +17835,7 @@
         <v>629</v>
       </c>
       <c r="M342" t="b">
-        <f>OR(K342&lt;&gt;L342,I342&lt;&gt;J342)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N342" t="s">
@@ -17849,7 +17868,7 @@
         <v>631</v>
       </c>
       <c r="M343" t="b">
-        <f>OR(K343&lt;&gt;L343,I343&lt;&gt;J343)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N343" t="s">
@@ -17882,7 +17901,7 @@
         <v>1085</v>
       </c>
       <c r="M344" t="b">
-        <f>OR(K344&lt;&gt;L344,I344&lt;&gt;J344)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N344" t="s">
@@ -17915,7 +17934,7 @@
         <v>1087</v>
       </c>
       <c r="M345" t="b">
-        <f>OR(K345&lt;&gt;L345,I345&lt;&gt;J345)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N345" t="s">
@@ -17948,7 +17967,7 @@
         <v>1089</v>
       </c>
       <c r="M346" t="b">
-        <f>OR(K346&lt;&gt;L346,I346&lt;&gt;J346)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N346" t="s">
@@ -17981,7 +18000,7 @@
         <v>1091</v>
       </c>
       <c r="M347" t="b">
-        <f>OR(K347&lt;&gt;L347,I347&lt;&gt;J347)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N347" t="s">
@@ -18014,7 +18033,7 @@
         <v>565</v>
       </c>
       <c r="M348" t="b">
-        <f>OR(K348&lt;&gt;L348,I348&lt;&gt;J348)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N348" t="s">
@@ -18047,7 +18066,7 @@
         <v>567</v>
       </c>
       <c r="M349" t="b">
-        <f>OR(K349&lt;&gt;L349,I349&lt;&gt;J349)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N349" t="s">
@@ -18080,7 +18099,7 @@
         <v>569</v>
       </c>
       <c r="M350" t="b">
-        <f>OR(K350&lt;&gt;L350,I350&lt;&gt;J350)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N350" t="s">
@@ -18113,7 +18132,7 @@
         <v>571</v>
       </c>
       <c r="M351" t="b">
-        <f>OR(K351&lt;&gt;L351,I351&lt;&gt;J351)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N351" t="s">
@@ -18146,7 +18165,7 @@
         <v>573</v>
       </c>
       <c r="M352" t="b">
-        <f>OR(K352&lt;&gt;L352,I352&lt;&gt;J352)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N352" t="s">
@@ -18179,7 +18198,7 @@
         <v>575</v>
       </c>
       <c r="M353" t="b">
-        <f>OR(K353&lt;&gt;L353,I353&lt;&gt;J353)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N353" t="s">
@@ -18212,7 +18231,7 @@
         <v>577</v>
       </c>
       <c r="M354" t="b">
-        <f>OR(K354&lt;&gt;L354,I354&lt;&gt;J354)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N354" t="s">
@@ -18245,7 +18264,7 @@
         <v>579</v>
       </c>
       <c r="M355" t="b">
-        <f>OR(K355&lt;&gt;L355,I355&lt;&gt;J355)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N355" t="s">
@@ -18278,7 +18297,7 @@
         <v>582</v>
       </c>
       <c r="M356" t="b">
-        <f>OR(K356&lt;&gt;L356,I356&lt;&gt;J356)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N356" t="s">
@@ -18311,7 +18330,7 @@
         <v>584</v>
       </c>
       <c r="M357" t="b">
-        <f>OR(K357&lt;&gt;L357,I357&lt;&gt;J357)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N357" t="s">
@@ -18344,7 +18363,7 @@
         <v>1166</v>
       </c>
       <c r="M358" t="b">
-        <f>OR(K358&lt;&gt;L358,I358&lt;&gt;J358)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N358" t="s">
@@ -18377,7 +18396,7 @@
         <v>633</v>
       </c>
       <c r="M359" t="b">
-        <f>OR(K359&lt;&gt;L359,I359&lt;&gt;J359)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N359" t="s">
@@ -18410,7 +18429,7 @@
         <v>635</v>
       </c>
       <c r="M360" t="b">
-        <f>OR(K360&lt;&gt;L360,I360&lt;&gt;J360)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N360" t="s">
@@ -18443,7 +18462,7 @@
         <v>924</v>
       </c>
       <c r="M361" t="b">
-        <f>OR(K361&lt;&gt;L361,I361&lt;&gt;J361)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N361" t="s">
@@ -18457,6 +18476,30 @@
       </c>
       <c r="Q361" t="s">
         <v>833</v>
+      </c>
+    </row>
+    <row r="362" spans="8:17" ht="15">
+      <c r="H362" t="s">
+        <v>586</v>
+      </c>
+      <c r="I362" t="s">
+        <v>830</v>
+      </c>
+      <c r="J362" t="s">
+        <v>830</v>
+      </c>
+      <c r="K362" s="44" t="s">
+        <v>1690</v>
+      </c>
+      <c r="L362" s="44" t="s">
+        <v>1690</v>
+      </c>
+      <c r="M362" t="b">
+        <f t="shared" ref="M362" si="6">OR(K362&lt;&gt;L362,I362&lt;&gt;J362)</f>
+        <v>0</v>
+      </c>
+      <c r="N362" t="s">
+        <v>1691</v>
       </c>
     </row>
   </sheetData>
@@ -18464,7 +18507,7 @@
     <sortCondition ref="K3"/>
   </sortState>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24624,7 +24667,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>440</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -24635,7 +24678,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="44"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="10" t="s">
         <v>441</v>
       </c>
@@ -24644,7 +24687,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="44"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="10" t="s">
         <v>442</v>
       </c>
@@ -24653,7 +24696,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="44"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="10" t="s">
         <v>443</v>
       </c>
@@ -24662,7 +24705,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="44"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="10" t="s">
         <v>444</v>
       </c>
@@ -24671,7 +24714,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="44"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="10" t="s">
         <v>445</v>
       </c>
@@ -24680,7 +24723,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="44"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="10" t="s">
         <v>446</v>
       </c>
@@ -24689,7 +24732,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>448</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -24700,7 +24743,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="44"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="10" t="s">
         <v>449</v>
       </c>
@@ -24709,7 +24752,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="44"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="10" t="s">
         <v>450</v>
       </c>
@@ -24718,7 +24761,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="44"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="10" t="s">
         <v>451</v>
       </c>
@@ -24727,7 +24770,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="44"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="10" t="s">
         <v>452</v>
       </c>
@@ -24736,7 +24779,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="46" t="s">
         <v>454</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -24747,7 +24790,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="44"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="10" t="s">
         <v>455</v>
       </c>
@@ -24756,7 +24799,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="44"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="10" t="s">
         <v>456</v>
       </c>
@@ -24765,7 +24808,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="44"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="10" t="s">
         <v>457</v>
       </c>
@@ -24774,7 +24817,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="44"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="10" t="s">
         <v>458</v>
       </c>
@@ -24805,7 +24848,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="46" t="s">
         <v>464</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -24816,7 +24859,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="44"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="10" t="s">
         <v>465</v>
       </c>
@@ -24825,7 +24868,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="46" t="s">
         <v>467</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -24836,7 +24879,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="44"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="10" t="s">
         <v>468</v>
       </c>
@@ -24845,7 +24888,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="44"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="10" t="s">
         <v>469</v>
       </c>

</xml_diff>